<commit_message>
update before rearranging folder layout to fit the style of other assays better
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonweirather/Source/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonweirather/Dropbox (Partners HealthCare)/projects/2019_05_CIDC-json-schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D991AE-5AE4-054D-B0D6-3309C5A4021B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065E6603-C7DA-B948-BEB1-76520D1C6EFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
@@ -63,19 +63,6 @@
             <family val="2"/>
           </rPr>
           <t>Artifact category.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Assay category.</t>
         </r>
       </text>
     </comment>
@@ -252,6 +239,39 @@
     <t>Immunity</t>
   </si>
   <si>
+    <t>run1a.fcs,run1b.fcs</t>
+  </si>
+  <si>
+    <t>CYTOF-9000</t>
+  </si>
+  <si>
+    <t>ABCDF</t>
+  </si>
+  <si>
+    <t>MA036-001</t>
+  </si>
+  <si>
+    <t>MA036-001 PRE</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>sample1.fcs</t>
+  </si>
+  <si>
+    <t>sample1a.fcs,sample1b.fcs</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>142Nd,143Nd,144Nd</t>
+  </si>
+  <si>
     <t>CD8</t>
   </si>
   <si>
@@ -265,39 +285,6 @@
   </si>
   <si>
     <t>146Nd</t>
-  </si>
-  <si>
-    <t>MA036-001</t>
-  </si>
-  <si>
-    <t>MA036-001 PRE</t>
-  </si>
-  <si>
-    <t>PRE</t>
-  </si>
-  <si>
-    <t>sample1.fcs</t>
-  </si>
-  <si>
-    <t>sample1a.fcs,sample1b.fcs</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>142Nd,143Nd,144Nd</t>
-  </si>
-  <si>
-    <t>run1a.fcs,run1b.fcs</t>
-  </si>
-  <si>
-    <t>CYTOF-9000</t>
-  </si>
-  <si>
-    <t>ABCDF</t>
   </si>
 </sst>
 </file>
@@ -411,13 +398,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -894,16 +881,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="6">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4">
         <v>43319</v>
       </c>
       <c r="D10" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1913,10 +1900,10 @@
     <mergeCell ref="B8:G8"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{AAB1D499-040B-2E44-8189-E566C12DE86A}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{0A1EE308-2807-454A-9D70-53339D2F1BB5}">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1929,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1996,20 +1983,20 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>46</v>
-      </c>
-      <c r="E3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2018,13 +2005,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="J3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3043,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3091,22 +3078,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update for directory structure
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonweirather/Dropbox (Partners HealthCare)/projects/2019_05_CIDC-json-schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065E6603-C7DA-B948-BEB1-76520D1C6EFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB89190-4162-2C40-A0BD-94CE4A8F5544}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-46120" yWindow="9080" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>The name of the center that created this artificat</t>
+          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
@@ -49,11 +49,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Indicates what site is filling out the assay</t>
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -131,18 +131,18 @@
     <t>#p</t>
   </si>
   <si>
-    <t>CREATOR</t>
-  </si>
-  <si>
     <t>LEAD ORGANIZATION STUDY ID</t>
   </si>
   <si>
+    <t>ASSAY CREATOR</t>
+  </si>
+  <si>
+    <t>ASSAY_CATEGORY</t>
+  </si>
+  <si>
     <t>ARTIFACT_CATEGORY</t>
   </si>
   <si>
-    <t>ASSAY_CATEGORY</t>
-  </si>
-  <si>
     <t>PANEL NAME</t>
   </si>
   <si>
@@ -227,7 +227,7 @@
     <t>ISOTOPE</t>
   </si>
   <si>
-    <t>Jon Doe</t>
+    <t>DFCI</t>
   </si>
   <si>
     <t>Assay Artifact from CIMAC</t>
@@ -236,7 +236,7 @@
     <t>CyTOF</t>
   </si>
   <si>
-    <t>Immunity</t>
+    <t>Immune-1</t>
   </si>
   <si>
     <t>run1a.fcs,run1b.fcs</t>
@@ -775,8 +775,8 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>35</v>
+      <c r="C2" s="1">
+        <v>10021</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -790,8 +790,8 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
-        <v>10021</v>
+      <c r="C3" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -806,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -821,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1899,11 +1899,14 @@
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B8:G8"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{AAB1D499-040B-2E44-8189-E566C12DE86A}">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{E2302947-2357-A844-BB28-FB24C58A14F7}">
+      <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{90DF5B84-40C7-134C-BE8A-CBB9C48A5D58}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{0A1EE308-2807-454A-9D70-53339D2F1BB5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{32E9B17D-B78A-3A40-B979-05A9283922A4}">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3031,7 +3034,7 @@
   <dimension ref="A1:G202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add a validating example
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonweirather/Dropbox (Partners HealthCare)/projects/2019_05_CIDC-json-schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB89190-4162-2C40-A0BD-94CE4A8F5544}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9BCCF7-305F-C142-B944-B4F91586518F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-46120" yWindow="9080" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Assay category.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -137,10 +150,10 @@
     <t>ASSAY CREATOR</t>
   </si>
   <si>
-    <t>ASSAY_CATEGORY</t>
-  </si>
-  <si>
-    <t>ARTIFACT_CATEGORY</t>
+    <t>ASSAY CATEGORY</t>
+  </si>
+  <si>
+    <t>ARTIFACT CATEGORY</t>
   </si>
   <si>
     <t>PANEL NAME</t>
@@ -227,25 +240,25 @@
     <t>ISOTOPE</t>
   </si>
   <si>
+    <t>run1a.fcs,run1b.fcs</t>
+  </si>
+  <si>
+    <t>CYTOF-9000</t>
+  </si>
+  <si>
+    <t>ABCDF</t>
+  </si>
+  <si>
     <t>DFCI</t>
   </si>
   <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
     <t>Assay Artifact from CIMAC</t>
   </si>
   <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
     <t>Immune-1</t>
-  </si>
-  <si>
-    <t>run1a.fcs,run1b.fcs</t>
-  </si>
-  <si>
-    <t>CYTOF-9000</t>
-  </si>
-  <si>
-    <t>ABCDF</t>
   </si>
   <si>
     <t>MA036-001</t>
@@ -746,7 +759,7 @@
   <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:G10"/>
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -791,7 +804,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -806,7 +819,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -821,7 +834,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -836,7 +849,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -881,16 +894,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C10" s="4">
         <v>43319</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1900,14 +1913,14 @@
     <mergeCell ref="B8:G8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{E2302947-2357-A844-BB28-FB24C58A14F7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{404DC2E0-CCC5-F144-AB25-61DBCC41184B}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{90DF5B84-40C7-134C-BE8A-CBB9C48A5D58}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{23EF6004-06E8-0548-8AF9-609B3DD58F05}">
+      <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{39E50FBA-AFAA-0042-A7C7-9B8216727D43}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{32E9B17D-B78A-3A40-B979-05A9283922A4}">
-      <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add some redundant data so we can more exactly fit the template example
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonweirather/Dropbox (Partners HealthCare)/projects/2019_05_CIDC-json-schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E9BCCF7-305F-C142-B944-B4F91586518F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FE5CD2-9E72-394E-BA98-5279EB6E8388}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,7 +89,20 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -132,8 +145,31 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>CIDC</author>
+  </authors>
+  <commentList>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="55">
   <si>
     <t>#t</t>
   </si>
@@ -240,6 +276,18 @@
     <t>ISOTOPE</t>
   </si>
   <si>
+    <t>DFCI</t>
+  </si>
+  <si>
+    <t>CyTOF</t>
+  </si>
+  <si>
+    <t>Assay Artifact from CIMAC</t>
+  </si>
+  <si>
+    <t>Immune-1</t>
+  </si>
+  <si>
     <t>run1a.fcs,run1b.fcs</t>
   </si>
   <si>
@@ -247,18 +295,6 @@
   </si>
   <si>
     <t>ABCDF</t>
-  </si>
-  <si>
-    <t>DFCI</t>
-  </si>
-  <si>
-    <t>CyTOF</t>
-  </si>
-  <si>
-    <t>Assay Artifact from CIMAC</t>
-  </si>
-  <si>
-    <t>Immune-1</t>
   </si>
   <si>
     <t>MA036-001</t>
@@ -759,7 +795,7 @@
   <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -804,7 +840,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -819,7 +855,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -834,7 +870,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -849,7 +885,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -894,16 +930,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C10" s="4">
         <v>43319</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1913,13 +1949,13 @@
     <mergeCell ref="B8:G8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{404DC2E0-CCC5-F144-AB25-61DBCC41184B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{14E539FE-42A1-CC48-ACCC-E445AFB819E0}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{23EF6004-06E8-0548-8AF9-609B3DD58F05}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{05C82FC8-04B3-0840-9DC4-98D4F9EB4FAD}">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{39E50FBA-AFAA-0042-A7C7-9B8216727D43}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{8CD9C97C-C9A0-5E49-A6B9-12C76F8CFD52}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1930,10 +1966,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L202"/>
+  <dimension ref="A1:L204"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1942,106 +1978,116 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1">
+        <v>10021</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
+      <c r="B5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3028,12 +3074,22 @@
         <v>10</v>
       </c>
     </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B3:L3"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I204" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3043,11 +3099,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G202"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:L204"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3056,123 +3112,133 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1">
+        <v>10021</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D5" t="s">
         <v>52</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="F3">
+      <c r="F5">
         <v>3983272</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4107,10 +4173,21 @@
         <v>10</v>
       </c>
     </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
seems that wasn't the lack of the study causing the issue
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonweirather/Dropbox (Partners HealthCare)/projects/2019_05_CIDC-json-schema/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FE5CD2-9E72-394E-BA98-5279EB6E8388}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91F475D-23C9-5647-81A0-10FF61195BBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,20 +89,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -115,7 +102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -128,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -145,31 +132,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>CIDC</author>
-  </authors>
-  <commentList>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="55">
   <si>
     <t>#t</t>
   </si>
@@ -795,7 +759,7 @@
   <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B10" sqref="B10:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1949,13 +1913,13 @@
     <mergeCell ref="B8:G8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{14E539FE-42A1-CC48-ACCC-E445AFB819E0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{EA9F6E37-09BB-A245-A7DE-188A117E68BC}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{05C82FC8-04B3-0840-9DC4-98D4F9EB4FAD}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{F77ECB3A-1CD0-274B-8C9B-984F0724CE61}">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{8CD9C97C-C9A0-5E49-A6B9-12C76F8CFD52}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{7AF98DC0-7B73-0740-9B51-B01023164C0E}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1966,10 +1930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:L204"/>
+  <dimension ref="A1:L202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B3" sqref="B3:L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1978,116 +1942,106 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1">
-        <v>10021</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
-        <v>47</v>
-      </c>
-      <c r="J5" t="s">
-        <v>48</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -3074,22 +3028,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I204" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3099,11 +3043,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L204"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3112,133 +3056,123 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1">
-        <v>10021</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3">
+        <v>3983272</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5">
-        <v>3983272</v>
-      </c>
-      <c r="G5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4173,21 +4107,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A203" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A204" t="s">
-        <v>10</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to cytof schemas
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonweirather/Dropbox (Partners HealthCare)/projects/2019_05_CIDC-json-schema/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91F475D-23C9-5647-81A0-10FF61195BBE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FBD043-F092-DA4D-8EC8-584E4668B3B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1120" yWindow="-20100" windowWidth="24220" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
@@ -758,7 +758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G209"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B10" sqref="B10:G10"/>
     </sheetView>
   </sheetViews>
@@ -1913,13 +1913,13 @@
     <mergeCell ref="B8:G8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{EA9F6E37-09BB-A245-A7DE-188A117E68BC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{F77ECB3A-1CD0-274B-8C9B-984F0724CE61}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{7AF98DC0-7B73-0740-9B51-B01023164C0E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3046,8 +3046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edits made to naming conventions and references
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FBD043-F092-DA4D-8EC8-584E4668B3B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E633F51A-5CFA-2F41-B358-AD46CFF11D6F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1120" yWindow="-20100" windowWidth="24220" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="800" yWindow="-17580" windowWidth="22380" windowHeight="12520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="54">
   <si>
     <t>#t</t>
   </si>
@@ -180,10 +180,10 @@
     <t>INJECTOR</t>
   </si>
   <si>
-    <t>ACQUISITION_BUFFER</t>
-  </si>
-  <si>
-    <t>BATCH_ID</t>
+    <t>ACQUISITION BUFFER</t>
+  </si>
+  <si>
+    <t>BATCH ID</t>
   </si>
   <si>
     <t>Samples</t>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>DEBARCODING KEY</t>
-  </si>
-  <si>
-    <t>BATCH ID</t>
   </si>
   <si>
     <t>TARGET</t>
@@ -804,7 +801,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -819,7 +816,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -834,7 +831,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -849,7 +846,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -894,16 +891,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="4">
         <v>43319</v>
       </c>
       <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
         <v>40</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -1992,7 +1989,7 @@
         <v>27</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2000,19 +1997,19 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>44</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2021,13 +2018,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" t="s">
         <v>47</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3071,22 +3068,22 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -3094,22 +3091,22 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Cytof working group feedback
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priti/Documents/GIT/schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FBD043-F092-DA4D-8EC8-584E4668B3B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6542AF0F-22ED-6A47-A4FE-B5412FBBDF1D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1120" yWindow="-20100" windowWidth="24220" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57880" yWindow="4800" windowWidth="35520" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="64">
   <si>
     <t>#t</t>
   </si>
@@ -186,6 +186,15 @@
     <t>BATCH_ID</t>
   </si>
   <si>
+    <t>AVERAGE_EVENT_PER_SECOND</t>
+  </si>
+  <si>
+    <t>RUN_TIME</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
     <t>Samples</t>
   </si>
   <si>
@@ -240,6 +249,12 @@
     <t>ISOTOPE</t>
   </si>
   <si>
+    <t>DILUTION</t>
+  </si>
+  <si>
+    <t>STAIN_TYPE</t>
+  </si>
+  <si>
     <t>DFCI</t>
   </si>
   <si>
@@ -261,6 +276,33 @@
     <t>ABCDF</t>
   </si>
   <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Clog at minute 20, washed machine and re started sample</t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>146Nd</t>
+  </si>
+  <si>
+    <t>100X</t>
+  </si>
+  <si>
+    <t>Surface Stain</t>
+  </si>
+  <si>
     <t>MA036-001</t>
   </si>
   <si>
@@ -283,21 +325,6 @@
   </si>
   <si>
     <t>142Nd,143Nd,144Nd</t>
-  </si>
-  <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>146Nd</t>
   </si>
 </sst>
 </file>
@@ -756,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G209"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:G10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -768,7 +795,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -780,8 +807,11 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -795,8 +825,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -804,14 +837,17 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -819,14 +855,17 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -834,14 +873,17 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -849,14 +891,17 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -865,8 +910,11 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -888,22 +936,31 @@
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4">
         <v>43319</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -911,33 +968,42 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>4567</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1909,17 +1975,17 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B8:J8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{D6E0765D-7409-5D42-B48B-605D67C6196B}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{5066DCFF-4D21-B54C-B4D9-F8866D52BBD2}">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{51CDFEB1-8F1E-294A-ABC7-A95B5419AC76}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1932,7 +1998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:L3"/>
     </sheetView>
   </sheetViews>
@@ -1944,7 +2010,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1962,37 +2028,37 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2000,19 +2066,19 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2021,13 +2087,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3044,10 +3110,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:I202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3056,123 +3122,137 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4109,8 +4189,13 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>"Surface Stain,Intracellular"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cytof working group feedback (#58)
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priti/Documents/GIT/schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FBD043-F092-DA4D-8EC8-584E4668B3B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6542AF0F-22ED-6A47-A4FE-B5412FBBDF1D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1120" yWindow="-20100" windowWidth="24220" windowHeight="12440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57880" yWindow="4800" windowWidth="35520" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="64">
   <si>
     <t>#t</t>
   </si>
@@ -186,6 +186,15 @@
     <t>BATCH_ID</t>
   </si>
   <si>
+    <t>AVERAGE_EVENT_PER_SECOND</t>
+  </si>
+  <si>
+    <t>RUN_TIME</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
     <t>Samples</t>
   </si>
   <si>
@@ -240,6 +249,12 @@
     <t>ISOTOPE</t>
   </si>
   <si>
+    <t>DILUTION</t>
+  </si>
+  <si>
+    <t>STAIN_TYPE</t>
+  </si>
+  <si>
     <t>DFCI</t>
   </si>
   <si>
@@ -261,6 +276,33 @@
     <t>ABCDF</t>
   </si>
   <si>
+    <t>30 minutes</t>
+  </si>
+  <si>
+    <t>Clog at minute 20, washed machine and re started sample</t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>146Nd</t>
+  </si>
+  <si>
+    <t>100X</t>
+  </si>
+  <si>
+    <t>Surface Stain</t>
+  </si>
+  <si>
     <t>MA036-001</t>
   </si>
   <si>
@@ -283,21 +325,6 @@
   </si>
   <si>
     <t>142Nd,143Nd,144Nd</t>
-  </si>
-  <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>146Nd</t>
   </si>
 </sst>
 </file>
@@ -756,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G209"/>
+  <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:G10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -768,7 +795,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -780,8 +807,11 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -795,8 +825,11 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -804,14 +837,17 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -819,14 +855,17 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -834,14 +873,17 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -849,14 +891,17 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
@@ -865,8 +910,11 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -888,22 +936,31 @@
       <c r="G9" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="C10" s="4">
         <v>43319</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -911,33 +968,42 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10">
+        <v>4567</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1909,17 +1975,17 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B1:J1"/>
+    <mergeCell ref="B8:J8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{D6E0765D-7409-5D42-B48B-605D67C6196B}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{5066DCFF-4D21-B54C-B4D9-F8866D52BBD2}">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{51CDFEB1-8F1E-294A-ABC7-A95B5419AC76}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1932,7 +1998,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:L3"/>
     </sheetView>
   </sheetViews>
@@ -1944,7 +2010,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -1962,37 +2028,37 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2000,19 +2066,19 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2021,13 +2087,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="J3" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3044,10 +3110,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:I202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:G3"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3056,123 +3122,137 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4109,8 +4189,13 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000000000000}">
+      <formula1>"Surface Stain,Intracellular"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edits to naming conventions, assay references, and artifact creations
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priti/Documents/GIT/schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dnunes/cidc-schemas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6542AF0F-22ED-6A47-A4FE-B5412FBBDF1D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51FF6B5E-7A16-584B-B94B-75E903D6A55B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57880" yWindow="4800" windowWidth="35520" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2080" yWindow="-19120" windowWidth="25880" windowHeight="15900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="63">
   <si>
     <t>#t</t>
   </si>
@@ -180,16 +180,16 @@
     <t>INJECTOR</t>
   </si>
   <si>
-    <t>ACQUISITION_BUFFER</t>
-  </si>
-  <si>
-    <t>BATCH_ID</t>
-  </si>
-  <si>
-    <t>AVERAGE_EVENT_PER_SECOND</t>
-  </si>
-  <si>
-    <t>RUN_TIME</t>
+    <t>ACQUISITION BUFFER</t>
+  </si>
+  <si>
+    <t>BATCH ID</t>
+  </si>
+  <si>
+    <t>AVERAGE EVENT PER SECOND</t>
+  </si>
+  <si>
+    <t>RUN TIME</t>
   </si>
   <si>
     <t>NOTES</t>
@@ -228,9 +228,6 @@
     <t>DEBARCODING KEY</t>
   </si>
   <si>
-    <t>BATCH ID</t>
-  </si>
-  <si>
     <t>TARGET</t>
   </si>
   <si>
@@ -252,7 +249,7 @@
     <t>DILUTION</t>
   </si>
   <si>
-    <t>STAIN_TYPE</t>
+    <t>STAIN TYPE</t>
   </si>
   <si>
     <t>DFCI</t>
@@ -282,6 +279,30 @@
     <t>Clog at minute 20, washed machine and re started sample</t>
   </si>
   <si>
+    <t>MA036-001</t>
+  </si>
+  <si>
+    <t>MA036-001 PRE</t>
+  </si>
+  <si>
+    <t>PRE</t>
+  </si>
+  <si>
+    <t>sample1.fcs</t>
+  </si>
+  <si>
+    <t>sample1a.fcs,sample1b.fcs</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>142Nd,143Nd,144Nd</t>
+  </si>
+  <si>
     <t>CD8</t>
   </si>
   <si>
@@ -301,30 +322,6 @@
   </si>
   <si>
     <t>Surface Stain</t>
-  </si>
-  <si>
-    <t>MA036-001</t>
-  </si>
-  <si>
-    <t>MA036-001 PRE</t>
-  </si>
-  <si>
-    <t>PRE</t>
-  </si>
-  <si>
-    <t>sample1.fcs</t>
-  </si>
-  <si>
-    <t>sample1a.fcs,sample1b.fcs</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>default</t>
-  </si>
-  <si>
-    <t>142Nd,143Nd,144Nd</t>
   </si>
 </sst>
 </file>
@@ -785,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J209"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -837,7 +834,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -855,7 +852,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -873,7 +870,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -891,7 +888,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -951,16 +948,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="4">
         <v>43319</v>
       </c>
       <c r="D10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" t="s">
         <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -972,10 +969,10 @@
         <v>4567</v>
       </c>
       <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" t="s">
         <v>47</v>
-      </c>
-      <c r="J10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1979,13 +1976,13 @@
     <mergeCell ref="B8:J8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{D6E0765D-7409-5D42-B48B-605D67C6196B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{5066DCFF-4D21-B54C-B4D9-F8866D52BBD2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{51CDFEB1-8F1E-294A-ABC7-A95B5419AC76}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1998,7 +1995,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:L3"/>
     </sheetView>
   </sheetViews>
@@ -2058,7 +2055,7 @@
         <v>30</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -2066,19 +2063,19 @@
         <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D3" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2087,13 +2084,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3113,7 +3110,7 @@
   <dimension ref="A1:I202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B3" sqref="B3:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3139,28 +3136,28 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3168,28 +3165,28 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="H3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
resolved typo error and updated docs
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,33 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priti/Documents/GIT/schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6542AF0F-22ED-6A47-A4FE-B5412FBBDF1D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57880" yWindow="4800" windowWidth="35520" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-43120" yWindow="5240" windowWidth="35520" windowHeight="20180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
     <sheet name="Data Preprocessing" sheetId="2" r:id="rId2"/>
     <sheet name="Antibody Information" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,12 +91,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -213,9 +220,6 @@
     <t>SOURCE FCS FILENAMES</t>
   </si>
   <si>
-    <t>CONCATONATION VERSION</t>
-  </si>
-  <si>
     <t>NORMALIZATION VERSION</t>
   </si>
   <si>
@@ -325,12 +329,15 @@
   </si>
   <si>
     <t>142Nd,143Nd,144Nd</t>
+  </si>
+  <si>
+    <t>CONCATENATION VERSION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -435,15 +442,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,9 +515,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -538,31 +545,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -590,23 +580,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -782,7 +755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J209"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -799,19 +772,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -829,7 +802,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -837,7 +810,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -847,7 +820,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -855,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -865,7 +838,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -873,7 +846,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -883,7 +856,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -891,7 +864,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -902,17 +875,17 @@
       <c r="J6" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -951,16 +924,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43319</v>
+      </c>
+      <c r="D10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="4">
-        <v>43319</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -972,10 +945,10 @@
         <v>4567</v>
       </c>
       <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" t="s">
         <v>47</v>
-      </c>
-      <c r="J10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1979,13 +1952,13 @@
     <mergeCell ref="B8:J8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{D6E0765D-7409-5D42-B48B-605D67C6196B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{5066DCFF-4D21-B54C-B4D9-F8866D52BBD2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{51CDFEB1-8F1E-294A-ABC7-A95B5419AC76}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1995,11 +1968,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2009,19 +1982,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2043,42 +2016,42 @@
         <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2087,13 +2060,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
         <v>61</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3099,7 +3072,7 @@
     <mergeCell ref="B1:L1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3109,7 +3082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -3123,44 +3096,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3168,28 +3141,28 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>52</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>54</v>
-      </c>
-      <c r="I3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4192,7 +4165,7 @@
     <mergeCell ref="B1:I1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
       <formula1>"Surface Stain,Intracellular"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated doc gen to work with new schema and updated latest docs (#106)
* updated doc gen to work with new schema and updated latest docs

* Edits and additions made to entity descriptions

* resolved typo error and updated docs
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,33 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/priti/Documents/GIT/schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6542AF0F-22ED-6A47-A4FE-B5412FBBDF1D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57880" yWindow="4800" windowWidth="35520" windowHeight="20180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-43120" yWindow="5240" windowWidth="35520" windowHeight="20180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
     <sheet name="Data Preprocessing" sheetId="2" r:id="rId2"/>
     <sheet name="Antibody Information" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="B5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -84,12 +91,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="B2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -115,7 +122,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="D2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -213,9 +220,6 @@
     <t>SOURCE FCS FILENAMES</t>
   </si>
   <si>
-    <t>CONCATONATION VERSION</t>
-  </si>
-  <si>
     <t>NORMALIZATION VERSION</t>
   </si>
   <si>
@@ -325,12 +329,15 @@
   </si>
   <si>
     <t>142Nd,143Nd,144Nd</t>
+  </si>
+  <si>
+    <t>CONCATENATION VERSION</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -435,15 +442,15 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,9 +515,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -538,31 +545,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -590,23 +580,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -782,7 +755,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J209"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -799,19 +772,19 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -829,7 +802,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -837,7 +810,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -847,7 +820,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -855,7 +828,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -865,7 +838,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -873,7 +846,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -883,7 +856,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -891,7 +864,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -902,17 +875,17 @@
       <c r="J6" s="1"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
@@ -951,16 +924,16 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="3">
+        <v>43319</v>
+      </c>
+      <c r="D10" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="4">
-        <v>43319</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>45</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -972,10 +945,10 @@
         <v>4567</v>
       </c>
       <c r="I10" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" t="s">
         <v>47</v>
-      </c>
-      <c r="J10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1979,13 +1952,13 @@
     <mergeCell ref="B8:J8"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{D6E0765D-7409-5D42-B48B-605D67C6196B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>"DFCI,Mount Sinai, Stanford, MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{5066DCFF-4D21-B54C-B4D9-F8866D52BBD2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
       <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{51CDFEB1-8F1E-294A-ABC7-A95B5419AC76}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
       <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1995,11 +1968,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2009,19 +1982,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2043,42 +2016,42 @@
         <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="D3" t="s">
         <v>57</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>58</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>59</v>
-      </c>
-      <c r="F3" t="s">
-        <v>60</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -2087,13 +2060,13 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" t="s">
         <v>61</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" s="5" t="s">
         <v>62</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -3099,7 +3072,7 @@
     <mergeCell ref="B1:L1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3109,7 +3082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -3123,44 +3096,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -3168,28 +3141,28 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>52</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H3" t="s">
         <v>53</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>54</v>
-      </c>
-      <c r="I3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4192,7 +4165,7 @@
     <mergeCell ref="B1:I1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
       <formula1>"Surface Stain,Intracellular"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
WIP cytof support in prism
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23300" windowHeight="14560" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23300" windowHeight="14560"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="62">
   <si>
     <t>#t</t>
   </si>
@@ -60,9 +60,6 @@
     <t>#d</t>
   </si>
   <si>
-    <t>CIMAC PARTICPANT ID</t>
-  </si>
-  <si>
     <t>CIMAC SAMPLE ID</t>
   </si>
   <si>
@@ -159,21 +156,12 @@
     <t>Y</t>
   </si>
   <si>
-    <t>default</t>
-  </si>
-  <si>
     <t>sample1.fcs</t>
   </si>
   <si>
     <t>Fluidigm 123</t>
   </si>
   <si>
-    <t>Fludign xyz</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
     <t>Fluidigm ZZTOP</t>
   </si>
   <si>
@@ -208,6 +196,24 @@
   </si>
   <si>
     <t>146Nb</t>
+  </si>
+  <si>
+    <t>CIMAC PARTICIPANT ID</t>
+  </si>
+  <si>
+    <t>CYTOF_TEST1</t>
+  </si>
+  <si>
+    <t>DFCI</t>
+  </si>
+  <si>
+    <t>IMMUNE4</t>
+  </si>
+  <si>
+    <t>XYZ1</t>
+  </si>
+  <si>
+    <t>FLUIDIGM XYZ</t>
   </si>
 </sst>
 </file>
@@ -332,9 +338,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -352,6 +355,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,8 +662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S207"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -670,26 +676,26 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -698,7 +704,9 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -723,7 +731,9 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -748,7 +758,9 @@
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -767,141 +779,141 @@
       <c r="S4" s="1"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3"/>
-      <c r="S6" s="3"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="O7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="P7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P7" s="2" t="s">
+      <c r="Q7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="Q7" s="2" t="s">
+      <c r="R7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="2" t="s">
+      <c r="S7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    </row>
+    <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="G8" s="7">
+        <v>43355</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="8">
-        <v>43355</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="I8" s="6">
+        <v>1</v>
+      </c>
+      <c r="J8" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="7">
-        <v>1</v>
-      </c>
-      <c r="I8" s="7" t="s">
+      <c r="K8" s="8">
+        <v>23</v>
+      </c>
+      <c r="L8" s="3">
+        <v>56</v>
+      </c>
+      <c r="M8" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="O8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K8" s="9">
-        <v>23</v>
-      </c>
-      <c r="L8" s="7">
-        <v>5</v>
-      </c>
-      <c r="M8" s="7" t="s">
+      <c r="P8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="R8" s="4">
+      <c r="S8" s="3">
         <v>1234</v>
       </c>
     </row>
@@ -1914,7 +1926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1925,102 +1937,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="B1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F3" s="3">
+        <v>3983272</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="4">
-        <v>3983272</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1231272</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1231272</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
WIP cytof support working, needs more unit tests
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="68">
   <si>
     <t>#t</t>
   </si>
@@ -214,6 +214,24 @@
   </si>
   <si>
     <t>FLUIDIGM XYZ</t>
+  </si>
+  <si>
+    <t>MA036-002</t>
+  </si>
+  <si>
+    <t>MA036-002 PRE</t>
+  </si>
+  <si>
+    <t>ABCY-MAD-A122</t>
+  </si>
+  <si>
+    <t>sample2.fcs</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>ZZABC</t>
   </si>
 </sst>
 </file>
@@ -662,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -901,6 +919,9 @@
       <c r="M8" s="6" t="s">
         <v>42</v>
       </c>
+      <c r="N8" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="O8" s="3" t="s">
         <v>43</v>
       </c>
@@ -920,6 +941,60 @@
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="7">
+        <v>43385</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="8">
+        <v>28</v>
+      </c>
+      <c r="L9" s="3">
+        <v>57</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
WIP cytof support, bug in artifact processing
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23300" windowHeight="14560"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23580" windowHeight="12960"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,418 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>CIDC</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Indicates what site is filling out the assay.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Standardized CyTOF panel name used for antibody sample development.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of CyTOF instrument on which experiment was conducted.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CyTOF batch identification number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Normalized CyTOF FCS filenames.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of CyTOF batch acquisition.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of Injector component used as part of the CyTOF software</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cell staining buffer used for antibody and cell dilution.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Analysis rate of CyTOF expressions per second.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Length of run time for CyTOF experiment.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Path to a file on a user's computer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Concatenation of FCS files into a single FCS version number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Version of normalization for CyTOF assay batch.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Confirmation of beads being removed after normalization process.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Protocol for the download and installation of the Debarcoder CyTOF software feature.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Key required for access to the Debarcoding software.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any notes pertaining to preprocessing of CyTOF data.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>CIDC</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody type collected for this study.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Resulting type of antibody clone from primary antibody sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Company from which antibody sample was derived.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody registry catalog number assigned to antibody sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identification number assigned to the particular quantity or lot of material from manufacturer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody isotype used to help differentiate antibody signals.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Concentration ratio of dilution buffer for primary antibody.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Type of staining method used for antibody.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>How this antibody should be used in automatic analysis</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="76">
   <si>
     <t>#t</t>
   </si>
@@ -48,6 +458,9 @@
     <t>PANEL NAME</t>
   </si>
   <si>
+    <t>INSTRUMENT</t>
+  </si>
+  <si>
     <t>Run info</t>
   </si>
   <si>
@@ -60,6 +473,9 @@
     <t>#d</t>
   </si>
   <si>
+    <t>CIMAC PARTICIPANT ID</t>
+  </si>
+  <si>
     <t>CIMAC SAMPLE ID</t>
   </si>
   <si>
@@ -75,9 +491,6 @@
     <t>DATE OF ACQUISITION</t>
   </si>
   <si>
-    <t>INSTRUMENT</t>
-  </si>
-  <si>
     <t>INJECTOR</t>
   </si>
   <si>
@@ -138,6 +551,60 @@
     <t>STAIN_TYPE</t>
   </si>
   <si>
+    <t>USAGE</t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>146Nd</t>
+  </si>
+  <si>
+    <t>100X</t>
+  </si>
+  <si>
+    <t>Surface Stain</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>C2/11p</t>
+  </si>
+  <si>
+    <t>C8-AB123</t>
+  </si>
+  <si>
+    <t>146Nb</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Analysis Only</t>
+  </si>
+  <si>
+    <t>CYTOF_TEST1</t>
+  </si>
+  <si>
+    <t>DFCI</t>
+  </si>
+  <si>
+    <t>IMMUNE4</t>
+  </si>
+  <si>
+    <t>PresNixon123</t>
+  </si>
+  <si>
     <t>MA036-001</t>
   </si>
   <si>
@@ -147,6 +614,9 @@
     <t>ABCY-MAD-A123</t>
   </si>
   <si>
+    <t>XYZ1</t>
+  </si>
+  <si>
     <t>sample1a.fcs,sample1b.fcs</t>
   </si>
   <si>
@@ -159,58 +629,7 @@
     <t>sample1.fcs</t>
   </si>
   <si>
-    <t>Fluidigm 123</t>
-  </si>
-  <si>
-    <t>Fluidigm ZZTOP</t>
-  </si>
-  <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>146Nd</t>
-  </si>
-  <si>
-    <t>100X</t>
-  </si>
-  <si>
-    <t>Surface Stain</t>
-  </si>
-  <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
-    <t>C2/11p</t>
-  </si>
-  <si>
-    <t>C8-AB123</t>
-  </si>
-  <si>
-    <t>146Nb</t>
-  </si>
-  <si>
-    <t>CIMAC PARTICIPANT ID</t>
-  </si>
-  <si>
-    <t>CYTOF_TEST1</t>
-  </si>
-  <si>
-    <t>DFCI</t>
-  </si>
-  <si>
-    <t>IMMUNE4</t>
-  </si>
-  <si>
-    <t>XYZ1</t>
+    <t>ABC</t>
   </si>
   <si>
     <t>FLUIDIGM XYZ</t>
@@ -228,10 +647,25 @@
     <t>sample2.fcs</t>
   </si>
   <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>ZZABC</t>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>GHIL</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>FLUIDIGM 1234</t>
+  </si>
+  <si>
+    <t>a note like any other note</t>
+  </si>
+  <si>
+    <t>a different note</t>
+  </si>
+  <si>
+    <t>sample2a.fcs,sample2b.fcs</t>
   </si>
 </sst>
 </file>
@@ -255,11 +689,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -288,7 +721,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -322,33 +755,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -357,21 +768,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -677,11 +1073,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S207"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -690,32 +1086,31 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -723,7 +1118,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -740,9 +1135,8 @@
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -750,7 +1144,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -767,9 +1161,8 @@
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -777,7 +1170,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -794,1215 +1187,1239 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="9" t="s">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9" t="s">
+      <c r="C5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" s="2" t="s">
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9">
+        <v>43355</v>
+      </c>
+      <c r="H9" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9">
+        <v>123</v>
+      </c>
+      <c r="K9">
         <v>23</v>
       </c>
-      <c r="Q7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="L9" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" t="s">
+        <v>70</v>
+      </c>
+      <c r="N9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O9" t="s">
+        <v>61</v>
+      </c>
+      <c r="P9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>72</v>
+      </c>
+      <c r="R9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10">
+        <v>43385</v>
+      </c>
+      <c r="H10" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="7">
-        <v>43355</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K8" s="8">
-        <v>23</v>
-      </c>
-      <c r="L8" s="3">
-        <v>56</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S8" s="3">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10">
+        <v>123</v>
+      </c>
+      <c r="K10">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>68</v>
+      </c>
+      <c r="M10" t="s">
+        <v>70</v>
+      </c>
+      <c r="N10" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="O10" t="s">
+        <v>71</v>
+      </c>
+      <c r="P10" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="7">
-        <v>43385</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="6">
-        <v>1</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K9" s="8">
-        <v>28</v>
-      </c>
-      <c r="L9" s="3">
-        <v>57</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="N9" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="Q10" t="s">
+        <v>72</v>
+      </c>
+      <c r="R10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:S1"/>
-    <mergeCell ref="B6:L6"/>
-    <mergeCell ref="M6:S6"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="B7:K7"/>
+    <mergeCell ref="L7:R7"/>
   </mergeCells>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O9:O208">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I202"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2011,1104 +2428,1118 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F3" s="3">
         <v>3983272</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="F4" s="3">
         <v>1231272</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I4">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
       <formula1>"Surface Stain,Intracellular"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202">
+      <formula1>"Ignored,Used,Analysis Only"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added cytof aliquot_id ref constraints support
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlindsay/Documents/Code/cidc/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA601672-34DF-4043-A95C-2864576C5976}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23580" windowHeight="12960"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="23580" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
     <sheet name="Antibody Information" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,12 +29,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -46,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B3" authorId="0">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B4" authorId="0">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -98,12 +99,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -111,7 +112,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -124,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -137,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -150,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -163,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -176,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -189,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0">
+    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -202,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K8" authorId="0">
+    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -215,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -228,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="0">
+    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -241,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0">
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -254,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -267,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0">
+    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -280,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="0">
+    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -293,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R8" authorId="0">
+    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -311,12 +312,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -329,7 +330,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -342,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -355,7 +356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -368,7 +369,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -381,7 +382,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -394,7 +395,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -407,7 +408,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -420,7 +421,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
+    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -605,15 +606,6 @@
     <t>PresNixon123</t>
   </si>
   <si>
-    <t>MA036-001</t>
-  </si>
-  <si>
-    <t>MA036-001 PRE</t>
-  </si>
-  <si>
-    <t>ABCY-MAD-A123</t>
-  </si>
-  <si>
     <t>XYZ1</t>
   </si>
   <si>
@@ -635,15 +627,6 @@
     <t>FLUIDIGM XYZ</t>
   </si>
   <si>
-    <t>MA036-002</t>
-  </si>
-  <si>
-    <t>MA036-002 PRE</t>
-  </si>
-  <si>
-    <t>ABCY-MAD-A122</t>
-  </si>
-  <si>
     <t>sample2.fcs</t>
   </si>
   <si>
@@ -666,13 +649,31 @@
   </si>
   <si>
     <t>sample2a.fcs,sample2b.fcs</t>
+  </si>
+  <si>
+    <t>test_AL_1.1.1</t>
+  </si>
+  <si>
+    <t>test_AL_1.2.1</t>
+  </si>
+  <si>
+    <t>test_SA_1.1</t>
+  </si>
+  <si>
+    <t>test_SA_2.1</t>
+  </si>
+  <si>
+    <t>test_PA_2</t>
+  </si>
+  <si>
+    <t>test_PA_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -691,6 +692,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -782,6 +789,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1073,11 +1083,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1110,7 +1120,7 @@
       <c r="Q1" s="4"/>
       <c r="R1" s="4"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1136,7 +1146,7 @@
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1162,7 +1172,7 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1188,7 +1198,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1298,28 +1308,28 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" t="s">
         <v>55</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
         <v>56</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F9" t="s">
-        <v>59</v>
       </c>
       <c r="G9">
         <v>43355</v>
       </c>
       <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
         <v>60</v>
-      </c>
-      <c r="I9" t="s">
-        <v>63</v>
       </c>
       <c r="J9">
         <v>123</v>
@@ -1328,25 +1338,25 @@
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="M9" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="N9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="O9" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" t="s">
         <v>61</v>
       </c>
-      <c r="P9" t="s">
-        <v>64</v>
-      </c>
       <c r="Q9" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="R9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
@@ -1354,28 +1364,28 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F10" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G10">
         <v>43385</v>
       </c>
       <c r="H10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I10" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="J10">
         <v>123</v>
@@ -1384,25 +1394,25 @@
         <v>28</v>
       </c>
       <c r="L10" t="s">
+        <v>62</v>
+      </c>
+      <c r="M10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" t="s">
+        <v>60</v>
+      </c>
+      <c r="O10" t="s">
+        <v>65</v>
+      </c>
+      <c r="P10" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>66</v>
+      </c>
+      <c r="R10" t="s">
         <v>68</v>
-      </c>
-      <c r="M10" t="s">
-        <v>70</v>
-      </c>
-      <c r="N10" t="s">
-        <v>63</v>
-      </c>
-      <c r="O10" t="s">
-        <v>71</v>
-      </c>
-      <c r="P10" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>72</v>
-      </c>
-      <c r="R10" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -2401,11 +2411,11 @@
     <mergeCell ref="B7:K7"/>
     <mergeCell ref="L7:R7"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O9:O208">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O9:O208" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2415,7 +2425,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J202"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -3532,10 +3542,10 @@
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Surface Stain,Intracellular"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Ignored,Used,Analysis Only"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed some tests wrt cimac_id
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA601672-34DF-4043-A95C-2864576C5976}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586F01BF-1667-8E4F-B2FA-FB08B1D785D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="23580" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,20 +86,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{034CBD05-8ECA-AF49-840A-408C838B0A75}">
       <text>
         <r>
           <rPr>
@@ -112,20 +99,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Aliquot identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{4D4356A5-C250-544D-AD5B-D5309CF2A52A}">
       <text>
         <r>
           <rPr>
@@ -138,12 +112,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{19CCAFB3-76BE-D548-8ABD-BA4DD7789D81}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -151,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{048D5500-05F1-F34F-B349-75872B8D0042}">
       <text>
         <r>
           <rPr>
@@ -164,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{F634914C-B114-A340-9DD2-20F1E6503F9C}">
       <text>
         <r>
           <rPr>
@@ -177,7 +151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{27AC1B77-C019-364B-A773-4BB911D92B72}">
       <text>
         <r>
           <rPr>
@@ -190,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{800D89CA-6D8F-CC4C-A30F-C636E0088D99}">
       <text>
         <r>
           <rPr>
@@ -203,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{05F8C5CB-ED31-954A-8A0A-8EECFF3C153A}">
       <text>
         <r>
           <rPr>
@@ -216,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{0B39990D-C464-F846-8709-EB20B5B4EA52}">
       <text>
         <r>
           <rPr>
@@ -229,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{368E07CF-12AD-FC4B-ABB5-116D8CF5B5A8}">
       <text>
         <r>
           <rPr>
@@ -242,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{81CD032F-241D-5345-9ED7-D57B61D37754}">
       <text>
         <r>
           <rPr>
@@ -255,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{125998E1-2B05-1143-AEDE-F87CB9C8DAA3}">
       <text>
         <r>
           <rPr>
@@ -268,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{EAF85C16-0190-4949-BBA0-D004EB59827F}">
       <text>
         <r>
           <rPr>
@@ -281,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{D2BAF493-A959-7A4D-86C6-BF06343D9970}">
       <text>
         <r>
           <rPr>
@@ -294,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{B04C048E-D431-E246-84C1-5037BA0EA868}">
       <text>
         <r>
           <rPr>
@@ -439,7 +413,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="70">
   <si>
     <t>#t</t>
   </si>
@@ -474,15 +448,6 @@
     <t>#d</t>
   </si>
   <si>
-    <t>CIMAC PARTICIPANT ID</t>
-  </si>
-  <si>
-    <t>CIMAC SAMPLE ID</t>
-  </si>
-  <si>
-    <t>CIMAC ALIQUOT ID</t>
-  </si>
-  <si>
     <t>BATCH_ID</t>
   </si>
   <si>
@@ -651,22 +616,13 @@
     <t>sample2a.fcs,sample2b.fcs</t>
   </si>
   <si>
-    <t>test_AL_1.1.1</t>
-  </si>
-  <si>
-    <t>test_AL_1.2.1</t>
-  </si>
-  <si>
-    <t>test_SA_1.1</t>
-  </si>
-  <si>
-    <t>test_SA_2.1</t>
-  </si>
-  <si>
-    <t>test_PA_2</t>
-  </si>
-  <si>
-    <t>test_PA_1</t>
+    <t>CIMAC ID</t>
+  </si>
+  <si>
+    <t>CM-TEST-PAR2-S1</t>
+  </si>
+  <si>
+    <t>CM-TEST-PAR1-S1</t>
   </si>
 </sst>
 </file>
@@ -1084,19 +1040,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R208"/>
+  <dimension ref="A1:P208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+    <col min="2" max="99" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1117,10 +1073,8 @@
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-    </row>
-    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1128,7 +1082,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1143,10 +1097,8 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1154,7 +1106,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1169,10 +1121,8 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-    </row>
-    <row r="4" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1180,7 +1130,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1195,10 +1145,8 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1206,7 +1154,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1221,10 +1169,8 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -1244,203 +1190,183 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="4"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R8" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9">
+        <v>43355</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9">
+        <v>123</v>
+      </c>
+      <c r="I9">
+        <v>23</v>
+      </c>
+      <c r="J9" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M9" t="s">
         <v>55</v>
       </c>
-      <c r="F9" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9">
-        <v>43355</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="N9" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10">
+        <v>43385</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10">
+        <v>123</v>
+      </c>
+      <c r="I10">
+        <v>28</v>
+      </c>
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" t="s">
         <v>57</v>
       </c>
-      <c r="I9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9">
-        <v>123</v>
-      </c>
-      <c r="K9">
-        <v>23</v>
-      </c>
-      <c r="L9" t="s">
-        <v>59</v>
-      </c>
-      <c r="M9" t="s">
-        <v>64</v>
-      </c>
-      <c r="N9" t="s">
-        <v>60</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="M10" t="s">
+        <v>62</v>
+      </c>
+      <c r="N10" t="s">
         <v>58</v>
       </c>
-      <c r="P9" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>66</v>
-      </c>
-      <c r="R9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>74</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10">
-        <v>43385</v>
-      </c>
-      <c r="H10" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="O10" t="s">
         <v>63</v>
       </c>
-      <c r="J10">
-        <v>123</v>
-      </c>
-      <c r="K10">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s">
-        <v>62</v>
-      </c>
-      <c r="M10" t="s">
-        <v>64</v>
-      </c>
-      <c r="N10" t="s">
-        <v>60</v>
-      </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>65</v>
       </c>
-      <c r="P10" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>66</v>
-      </c>
-      <c r="R10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -2407,15 +2333,15 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="B1:P1"/>
     <mergeCell ref="B7:K7"/>
-    <mergeCell ref="L7:R7"/>
+    <mergeCell ref="L7:P7"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O9:O208" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O11:O208 M9:M10" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2440,7 +2366,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2456,31 +2382,31 @@
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -2488,31 +2414,31 @@
         <v>10</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F3" s="3">
         <v>3983272</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -2520,31 +2446,31 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F4" s="3">
         <v>1231272</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed all tests and prism
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{586F01BF-1667-8E4F-B2FA-FB08B1D785D1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE772E6D-6075-274B-BAD8-1E45EE339045}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="23580" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -619,10 +619,10 @@
     <t>CIMAC ID</t>
   </si>
   <si>
-    <t>CM-TEST-PAR2-S1</t>
-  </si>
-  <si>
-    <t>CM-TEST-PAR1-S1</t>
+    <t>CM-TEST-PAR1-11</t>
+  </si>
+  <si>
+    <t>CM-TEST-PAR1-21</t>
   </si>
 </sst>
 </file>
@@ -1246,7 +1246,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
@@ -1296,7 +1296,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
protocol id -> identifier
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE772E6D-6075-274B-BAD8-1E45EE339045}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEA5C27-777C-6142-96D0-D958CA8BFD59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="23580" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -52,7 +52,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -424,9 +424,6 @@
     <t>#p</t>
   </si>
   <si>
-    <t>LEAD ORGANIZATION STUDY ID</t>
-  </si>
-  <si>
     <t>ASSAY CREATOR</t>
   </si>
   <si>
@@ -623,6 +620,9 @@
   </si>
   <si>
     <t>CM-TEST-PAR1-21</t>
+  </si>
+  <si>
+    <t>PROTOCOL IDENTIFIER</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1043,7 @@
   <dimension ref="A1:P208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1079,10 +1079,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1103,10 +1103,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1127,10 +1127,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1151,10 +1151,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1172,7 +1172,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -1184,7 +1184,7 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -1193,75 +1193,75 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="J8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="L8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N8" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
         <v>52</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
       </c>
       <c r="E9">
         <v>43355</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H9">
         <v>123</v>
@@ -1270,48 +1270,48 @@
         <v>23</v>
       </c>
       <c r="J9" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" t="s">
         <v>56</v>
       </c>
-      <c r="K9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" t="s">
         <v>57</v>
       </c>
-      <c r="M9" t="s">
-        <v>55</v>
-      </c>
-      <c r="N9" t="s">
-        <v>58</v>
-      </c>
       <c r="O9" t="s">
+        <v>62</v>
+      </c>
+      <c r="P9" t="s">
         <v>63</v>
-      </c>
-      <c r="P9" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E10">
         <v>43385</v>
       </c>
       <c r="F10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H10">
         <v>123</v>
@@ -1320,1015 +1320,1015 @@
         <v>28</v>
       </c>
       <c r="J10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M10" t="s">
         <v>61</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>57</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>62</v>
       </c>
-      <c r="N10" t="s">
-        <v>58</v>
-      </c>
-      <c r="O10" t="s">
-        <v>63</v>
-      </c>
       <c r="P10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -2366,7 +2366,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2379,1088 +2379,1088 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>38</v>
       </c>
       <c r="F3" s="3">
         <v>3983272</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="F4" s="3">
         <v>1231272</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="J4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cimac_id format update (#210)
* updated cimac_id & cimac_participant_id formats

* fixed cimac_id to cimac_participant_id parsing

* bump version to 0.9.0

* updated docs
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEA5C27-777C-6142-96D0-D958CA8BFD59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E805B7B2-5BA9-3D42-8B3A-1E66AB983E2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="23580" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1640" yWindow="960" windowWidth="23580" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -616,20 +616,20 @@
     <t>CIMAC ID</t>
   </si>
   <si>
-    <t>CM-TEST-PAR1-11</t>
-  </si>
-  <si>
-    <t>CM-TEST-PAR1-21</t>
-  </si>
-  <si>
     <t>PROTOCOL IDENTIFIER</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -655,6 +655,12 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -722,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -733,6 +739,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1043,7 +1050,7 @@
   <dimension ref="A1:P208"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1056,30 +1063,30 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>47</v>
@@ -1171,25 +1178,25 @@
       <c r="P5" s="1"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4" t="s">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1245,8 +1252,8 @@
       <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
-        <v>67</v>
+      <c r="B9" s="4" t="s">
+        <v>68</v>
       </c>
       <c r="C9" t="s">
         <v>51</v>
@@ -1295,8 +1302,8 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>68</v>
+      <c r="B10" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>
@@ -2346,6 +2353,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -2354,7 +2362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J202"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -2365,17 +2373,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
CyTOF Support: CyTOF Analysis Template (#216)
* created `cytof_analysis_template`
* added tests for `cytof_analysis_template`
* updated cytof xlsx templates
* bumped __version__ = '0.9.5'
* converged on test_prism_trial_id as the example template protocol identifier
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625FF66E-62F5-B34F-AB55-274625DE7B1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C6B77A-D6A8-8F43-9B11-D870F0304011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -31,11 +31,11 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>User defined unique identifier for this assay run.</t>
         </r>
       </text>
     </comment>
@@ -48,7 +48,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Indicates what site is filling out the assay.</t>
+          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
@@ -61,7 +61,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Standardized CyTOF panel name used for antibody sample development.</t>
+          <t>Indicates what site is filling out the assay.</t>
         </r>
       </text>
     </comment>
@@ -74,11 +74,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Standardized CyTOF panel name used for antibody sample development.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Name of CyTOF instrument on which experiment was conducted.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -91,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -117,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -130,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -143,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -156,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -169,7 +182,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +195,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +208,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -208,7 +221,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +234,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -247,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -260,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="P9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -405,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="72">
   <si>
     <t>#t</t>
   </si>
@@ -416,6 +429,9 @@
     <t>#p</t>
   </si>
   <si>
+    <t>Assay run id</t>
+  </si>
+  <si>
     <t>Protocol identifier</t>
   </si>
   <si>
@@ -515,9 +531,6 @@
     <t>Usage</t>
   </si>
   <si>
-    <t>CYTOF_TEST1</t>
-  </si>
-  <si>
     <t>DFCI</t>
   </si>
   <si>
@@ -615,13 +628,19 @@
   </si>
   <si>
     <t>Analysis Only</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id_run_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -645,12 +664,26 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -675,8 +708,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2D2F6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -710,11 +749,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
@@ -722,12 +770,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1067,10 +1121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P208"/>
+  <dimension ref="A1:P209"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B9" sqref="A9:XFD10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1083,25 +1137,25 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-    </row>
-    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1109,7 +1163,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -1125,15 +1179,15 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>37</v>
+      <c r="C3" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -1149,15 +1203,15 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>38</v>
+      <c r="C4" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -1173,15 +1227,15 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
     </row>
-    <row r="5" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>39</v>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -1197,157 +1251,131 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
+      <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="O8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D9" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9">
-        <v>43355</v>
-      </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9">
-        <v>123</v>
-      </c>
-      <c r="I9">
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J9" t="s">
-        <v>45</v>
-      </c>
-      <c r="K9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L9" t="s">
-        <v>44</v>
-      </c>
-      <c r="M9" t="s">
-        <v>47</v>
-      </c>
-      <c r="N9" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" t="s">
-        <v>49</v>
-      </c>
-      <c r="P9" t="s">
-        <v>50</v>
+      <c r="N9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>51</v>
+        <v>11</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E10">
-        <v>43385</v>
+        <v>43355</v>
       </c>
       <c r="F10" t="s">
         <v>43</v>
       </c>
       <c r="G10" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="H10">
         <v>123</v>
       </c>
       <c r="I10">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="K10" t="s">
         <v>46</v>
@@ -1356,7 +1384,7 @@
         <v>44</v>
       </c>
       <c r="M10" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="N10" t="s">
         <v>48</v>
@@ -1365,1010 +1393,1057 @@
         <v>49</v>
       </c>
       <c r="P10" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11">
+        <v>43385</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11">
+        <v>123</v>
+      </c>
+      <c r="I11">
+        <v>28</v>
+      </c>
+      <c r="J11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" t="s">
+        <v>44</v>
+      </c>
+      <c r="M11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" t="s">
+        <v>49</v>
+      </c>
+      <c r="P11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>10</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="J7:P7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="J8:P8"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{BE2BA306-6751-9B41-88A5-1E58868E7FDB}">
-      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M208" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M10:M209" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2382,7 +2457,7 @@
   <dimension ref="A1:J202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A3:XFD4"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2392,1102 +2467,1102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="B1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="6">
         <v>3983272</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="6" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="6">
         <v>1231272</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move batch_id to preamble section
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C6B77A-D6A8-8F43-9B11-D870F0304011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD255841-C746-2A41-8E51-E2BDD3351ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39260" yWindow="3540" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
     <sheet name="Antibody Information" sheetId="2" r:id="rId2"/>
+    <sheet name="Legend" sheetId="3" r:id="rId3"/>
+    <sheet name="Data Dictionary" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -31,7 +33,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -91,7 +93,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CyTOF batch identification number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -113,24 +128,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>CyTOF batch identification number.</t>
+          <t>Path to a file on a user's computer.
+In .fcs format</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a user's computer.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -143,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -156,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -169,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -204,11 +207,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.</t>
+          <t>Path to a file on a user's computer.
+In .fcs format</t>
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -247,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -260,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -273,12 +277,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="P9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -418,7 +422,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="120">
   <si>
     <t>#t</t>
   </si>
@@ -444,6 +448,9 @@
     <t>Instrument</t>
   </si>
   <si>
+    <t>Batch_id</t>
+  </si>
+  <si>
     <t>Run info</t>
   </si>
   <si>
@@ -459,9 +466,6 @@
     <t>Cimac id</t>
   </si>
   <si>
-    <t>Batch_id</t>
-  </si>
-  <si>
     <t>Original fcs filename(s)</t>
   </si>
   <si>
@@ -531,19 +535,187 @@
     <t>Usage</t>
   </si>
   <si>
+    <t>LEGEND</t>
+  </si>
+  <si>
+    <t>Legend for tab 'Acquisition and Preprocessing'</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>User defined unique identifier for this assay run.</t>
+  </si>
+  <si>
+    <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>Indicates what site is filling out the assay.</t>
+  </si>
+  <si>
+    <t>E.g. 'DFCI'</t>
+  </si>
+  <si>
+    <t>Standardized CyTOF panel name used for antibody sample development.</t>
+  </si>
+  <si>
+    <t>Name of CyTOF instrument on which experiment was conducted.</t>
+  </si>
+  <si>
+    <t>CyTOF batch identification number.</t>
+  </si>
+  <si>
+    <t>Section 'Run info' of tab 'Acquisition and Preprocessing'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String: regex ^C[A-Z0-9]{3}[A-Z0-9]{3}[A-Z0-9]{2}.[0-9]{2}$ </t>
+  </si>
+  <si>
+    <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+  </si>
+  <si>
+    <t>E.g. 'CTTTP01A1.00'</t>
+  </si>
+  <si>
+    <t>Path to a file on a user's computer.</t>
+  </si>
+  <si>
+    <t>Date of CyTOF batch acquisition.</t>
+  </si>
+  <si>
+    <t>Name of Injector component used as part of the CyTOF software</t>
+  </si>
+  <si>
+    <t>Cell staining buffer used for antibody and cell dilution.</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Analysis rate of CyTOF expressions per second.</t>
+  </si>
+  <si>
+    <t>Length of run time for CyTOF experiment.</t>
+  </si>
+  <si>
+    <t>Section 'Preprocessing' of tab 'Acquisition and Preprocessing'</t>
+  </si>
+  <si>
+    <t>Concatenation of FCS files into a single FCS version number.</t>
+  </si>
+  <si>
+    <t>Version of normalization for CyTOF assay batch.</t>
+  </si>
+  <si>
+    <t>Confirmation of beads being removed after normalization process.</t>
+  </si>
+  <si>
+    <t>E.g. 'Y'</t>
+  </si>
+  <si>
+    <t>Protocol for the download and installation of the Debarcoder CyTOF software feature.</t>
+  </si>
+  <si>
+    <t>Key required for access to the Debarcoding software.</t>
+  </si>
+  <si>
+    <t>Any notes pertaining to preprocessing of CyTOF data.</t>
+  </si>
+  <si>
+    <t>Legend for tab 'Antibody Information'</t>
+  </si>
+  <si>
+    <t>Section 'Samples' of tab 'Antibody Information'</t>
+  </si>
+  <si>
+    <t>Antibody type collected for this study.</t>
+  </si>
+  <si>
+    <t>Resulting type of antibody clone from primary antibody sample.</t>
+  </si>
+  <si>
+    <t>Company from which antibody sample was derived.</t>
+  </si>
+  <si>
+    <t>Antibody registry catalog number assigned to antibody sample.</t>
+  </si>
+  <si>
+    <t>Identification number assigned to the particular quantity or lot of material from manufacturer.</t>
+  </si>
+  <si>
+    <t>Antibody isotype used to help differentiate antibody signals.</t>
+  </si>
+  <si>
+    <t>Concentration ratio of dilution buffer for primary antibody.</t>
+  </si>
+  <si>
+    <t>Type of staining method used for antibody.</t>
+  </si>
+  <si>
+    <t>E.g. 'Surface Stain'</t>
+  </si>
+  <si>
+    <t>How this antibody should be used in automatic analysis</t>
+  </si>
+  <si>
+    <t>E.g. 'Ignored'</t>
+  </si>
+  <si>
     <t>DFCI</t>
   </si>
   <si>
+    <t>Mount Sinai</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>MD Anderson</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Surface Stain</t>
+  </si>
+  <si>
+    <t>Intracellular</t>
+  </si>
+  <si>
+    <t>Ignored</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Analysis Only</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id_run_1</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
     <t>IMMUNE4</t>
   </si>
   <si>
     <t>PresNixon123</t>
   </si>
   <si>
+    <t>XYZ1</t>
+  </si>
+  <si>
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>XYZ1</t>
+    <t>CTTTPP121.00</t>
   </si>
   <si>
     <t>sample1a.fcs,sample1b.fcs</t>
@@ -561,9 +733,6 @@
     <t>GHIL</t>
   </si>
   <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>FLUIDIGM XYZ</t>
   </si>
   <si>
@@ -573,9 +742,6 @@
     <t>a note like any other note</t>
   </si>
   <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
     <t>sample2a.fcs,sample2b.fcs</t>
   </si>
   <si>
@@ -585,9 +751,6 @@
     <t>sample2.fcs</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>a different note</t>
   </si>
   <si>
@@ -609,12 +772,6 @@
     <t>100X</t>
   </si>
   <si>
-    <t>Surface Stain</t>
-  </si>
-  <si>
-    <t>Used</t>
-  </si>
-  <si>
     <t>PD-L1</t>
   </si>
   <si>
@@ -625,15 +782,6 @@
   </si>
   <si>
     <t>146Nb</t>
-  </si>
-  <si>
-    <t>Analysis Only</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id_run_1</t>
   </si>
 </sst>
 </file>
@@ -683,7 +831,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -705,6 +853,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF5FA3F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -762,24 +916,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1121,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P209"/>
+  <dimension ref="A1:O210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1133,1317 +1290,1324 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+    </row>
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+    </row>
+    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="C6" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+    </row>
+    <row r="7" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
+      <c r="C7" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10">
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11">
         <v>43355</v>
       </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10">
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11">
         <v>123</v>
       </c>
-      <c r="I10">
+      <c r="H11">
         <v>23</v>
       </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M10" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" t="s">
-        <v>49</v>
-      </c>
-      <c r="P10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11">
+      <c r="I11" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" t="s">
+        <v>84</v>
+      </c>
+      <c r="M11" t="s">
+        <v>103</v>
+      </c>
+      <c r="N11" t="s">
+        <v>104</v>
+      </c>
+      <c r="O11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12">
         <v>43385</v>
       </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11">
+      <c r="E12" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" t="s">
+        <v>107</v>
+      </c>
+      <c r="G12">
         <v>123</v>
       </c>
-      <c r="I11">
+      <c r="H12">
         <v>28</v>
       </c>
-      <c r="J11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M11" t="s">
-        <v>55</v>
-      </c>
-      <c r="N11" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="I12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J12" t="s">
+        <v>102</v>
+      </c>
+      <c r="K12" t="s">
+        <v>100</v>
+      </c>
+      <c r="L12" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" t="s">
+        <v>103</v>
+      </c>
+      <c r="N12" t="s">
+        <v>104</v>
+      </c>
+      <c r="O12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="J8:P8"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B9:H9"/>
+    <mergeCell ref="I9:O9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M10:M209" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L11:L210" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2456,8 +2620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2467,1102 +2631,1102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="6">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3">
         <v>3983272</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>64</v>
+      <c r="G3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
+        <v>115</v>
+      </c>
+      <c r="I3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J3" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="6">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4">
         <v>1231272</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>69</v>
+      <c r="G4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J4" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3580,4 +3744,457 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:E35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>39</v>
+      </c>
+      <c r="D29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" t="s">
+        <v>78</v>
+      </c>
+      <c r="E35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
normalized & debarcoded fcs filename
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD255841-C746-2A41-8E51-E2BDD3351ECD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABEA7115-43E2-F64D-BED2-A41AD30093A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39260" yWindow="3540" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38980" yWindow="4500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -124,16 +124,48 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.
-In .fcs format</t>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
         </r>
       </text>
     </comment>
     <comment ref="D10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -146,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -159,7 +191,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -172,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -185,7 +217,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -198,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -212,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -238,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -251,7 +283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -264,7 +296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -277,12 +309,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="O10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="P10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -422,7 +454,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="605" uniqueCount="123">
   <si>
     <t>#t</t>
   </si>
@@ -466,7 +498,10 @@
     <t>Cimac id</t>
   </si>
   <si>
-    <t>Original fcs filename(s)</t>
+    <t>Raw fcs filename(s)</t>
+  </si>
+  <si>
+    <t>Normalized and debarcoded fcs filename</t>
   </si>
   <si>
     <t>Date of acquisition</t>
@@ -718,40 +753,46 @@
     <t>CTTTPP121.00</t>
   </si>
   <si>
+    <t>HAT123</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>sample1.fcs</t>
+  </si>
+  <si>
+    <t>GHIL</t>
+  </si>
+  <si>
+    <t>FLUIDIGM XYZ</t>
+  </si>
+  <si>
+    <t>FLUIDIGM 1234</t>
+  </si>
+  <si>
+    <t>a note like any other note</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>sample2.fcs</t>
+  </si>
+  <si>
+    <t>a different note</t>
+  </si>
+  <si>
     <t>sample1a.fcs,sample1b.fcs</t>
   </si>
   <si>
-    <t>HAT123</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>sample1.fcs</t>
-  </si>
-  <si>
-    <t>GHIL</t>
-  </si>
-  <si>
-    <t>FLUIDIGM XYZ</t>
-  </si>
-  <si>
-    <t>FLUIDIGM 1234</t>
-  </si>
-  <si>
-    <t>a note like any other note</t>
-  </si>
-  <si>
     <t>sample2a.fcs,sample2b.fcs</t>
   </si>
   <si>
-    <t>ABCD</t>
-  </si>
-  <si>
-    <t>sample2.fcs</t>
-  </si>
-  <si>
-    <t>a different note</t>
+    <t>sample1_n.fcs</t>
+  </si>
+  <si>
+    <t>sample2_n.fcs</t>
   </si>
   <si>
     <t>CD8</t>
@@ -811,12 +852,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -828,6 +863,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -916,7 +957,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -930,15 +971,18 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1278,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O210"/>
+  <dimension ref="A1:P210"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1290,28 +1334,29 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-    </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1319,7 +1364,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1333,16 +1378,17 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-    </row>
-    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P2" s="2"/>
+    </row>
+    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>92</v>
+      <c r="C3" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1356,16 +1402,17 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>80</v>
+      <c r="C4" s="7" t="s">
+        <v>81</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1379,16 +1426,17 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="2"/>
+    </row>
+    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>93</v>
+      <c r="C5" s="7" t="s">
+        <v>94</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1402,16 +1450,17 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-    </row>
-    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P5" s="2"/>
+    </row>
+    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>94</v>
+      <c r="C6" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1425,16 +1474,17 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-    </row>
-    <row r="7" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>95</v>
+      <c r="C7" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1448,28 +1498,30 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="8" t="s">
+      <c r="P7" s="2"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1515,117 +1567,126 @@
       <c r="O10" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P10" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>96</v>
+      <c r="B11" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="C11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11">
+        <v>43355</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" t="s">
+        <v>100</v>
+      </c>
+      <c r="H11">
+        <v>123</v>
+      </c>
+      <c r="I11">
+        <v>23</v>
+      </c>
+      <c r="J11" t="s">
+        <v>101</v>
+      </c>
+      <c r="K11" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" t="s">
+        <v>100</v>
+      </c>
+      <c r="M11" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" t="s">
+        <v>103</v>
+      </c>
+      <c r="O11" t="s">
+        <v>104</v>
+      </c>
+      <c r="P11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D11">
-        <v>43355</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="C12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12">
+        <v>43385</v>
+      </c>
+      <c r="F12" t="s">
         <v>99</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G12" t="s">
+        <v>106</v>
+      </c>
+      <c r="H12">
+        <v>123</v>
+      </c>
+      <c r="I12">
+        <v>28</v>
+      </c>
+      <c r="J12" t="s">
+        <v>107</v>
+      </c>
+      <c r="K12" t="s">
+        <v>102</v>
+      </c>
+      <c r="L12" t="s">
         <v>100</v>
       </c>
-      <c r="G11">
-        <v>123</v>
-      </c>
-      <c r="H11">
-        <v>23</v>
-      </c>
-      <c r="I11" t="s">
-        <v>101</v>
-      </c>
-      <c r="J11" t="s">
-        <v>102</v>
-      </c>
-      <c r="K11" t="s">
-        <v>100</v>
-      </c>
-      <c r="L11" t="s">
-        <v>84</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="M12" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" t="s">
         <v>103</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O12" t="s">
         <v>104</v>
       </c>
-      <c r="O11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C12" t="s">
-        <v>106</v>
-      </c>
-      <c r="D12">
-        <v>43385</v>
-      </c>
-      <c r="E12" t="s">
-        <v>99</v>
-      </c>
-      <c r="F12" t="s">
-        <v>107</v>
-      </c>
-      <c r="G12">
-        <v>123</v>
-      </c>
-      <c r="H12">
-        <v>28</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="P12" t="s">
         <v>108</v>
       </c>
-      <c r="J12" t="s">
-        <v>102</v>
-      </c>
-      <c r="K12" t="s">
-        <v>100</v>
-      </c>
-      <c r="L12" t="s">
-        <v>85</v>
-      </c>
-      <c r="M12" t="s">
-        <v>103</v>
-      </c>
-      <c r="N12" t="s">
-        <v>104</v>
-      </c>
-      <c r="O12" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2602,12 +2663,12 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:O1"/>
-    <mergeCell ref="B9:H9"/>
-    <mergeCell ref="I9:O9"/>
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="J9:P9"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L11:L210" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M11:M210" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2620,8 +2681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2631,112 +2692,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
+      <c r="B1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B3" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="F3">
+      <c r="C3" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="9">
         <v>3983272</v>
       </c>
-      <c r="G3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H3" t="s">
-        <v>115</v>
-      </c>
-      <c r="I3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" t="s">
-        <v>89</v>
+      <c r="G3" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" t="s">
-        <v>112</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B4" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1231272</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="H4" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F4">
-        <v>1231272</v>
-      </c>
-      <c r="G4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H4" t="s">
-        <v>115</v>
-      </c>
-      <c r="I4" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" t="s">
-        <v>90</v>
+      <c r="I4" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -3748,7 +3809,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="B1:E35"/>
+  <dimension ref="B1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3759,12 +3820,12 @@
   <sheetData>
     <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
       <c r="B1" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -3772,10 +3833,10 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -3783,10 +3844,10 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -3794,13 +3855,13 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -3808,10 +3869,10 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -3819,10 +3880,10 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
@@ -3830,15 +3891,15 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="32" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
@@ -3846,13 +3907,13 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -3860,10 +3921,10 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -3871,7 +3932,7 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D12" t="s">
         <v>53</v>
@@ -3882,7 +3943,7 @@
         <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
@@ -3893,7 +3954,7 @@
         <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>55</v>
@@ -3904,10 +3965,10 @@
         <v>18</v>
       </c>
       <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
         <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.2">
@@ -3915,26 +3976,26 @@
         <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="D16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>52</v>
+    <row r="18" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
@@ -3942,10 +4003,10 @@
         <v>21</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
@@ -3953,7 +4014,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>61</v>
@@ -3964,13 +4025,10 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
         <v>62</v>
-      </c>
-      <c r="E21" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
@@ -3978,9 +4036,12 @@
         <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3989,7 +4050,7 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D23" t="s">
         <v>65</v>
@@ -4000,14 +4061,20 @@
         <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
         <v>67</v>
       </c>
     </row>
@@ -4016,14 +4083,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" t="s">
+    <row r="27" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4032,7 +4093,7 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D28" t="s">
         <v>70</v>
@@ -4043,7 +4104,7 @@
         <v>30</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
         <v>71</v>
@@ -4054,7 +4115,7 @@
         <v>31</v>
       </c>
       <c r="C30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D30" t="s">
         <v>72</v>
@@ -4065,7 +4126,7 @@
         <v>32</v>
       </c>
       <c r="C31" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D31" t="s">
         <v>73</v>
@@ -4076,7 +4137,7 @@
         <v>33</v>
       </c>
       <c r="C32" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D32" t="s">
         <v>74</v>
@@ -4087,7 +4148,7 @@
         <v>34</v>
       </c>
       <c r="C33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D33" t="s">
         <v>75</v>
@@ -4098,13 +4159,10 @@
         <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D34" t="s">
         <v>76</v>
-      </c>
-      <c r="E34" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
@@ -4112,13 +4170,27 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" t="s">
         <v>78</v>
       </c>
-      <c r="E35" t="s">
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="s">
         <v>79</v>
+      </c>
+      <c r="E36" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -4143,54 +4215,54 @@
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cytof ct example
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5224D046-3935-3243-A1C2-EB15FC3F8047}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89596AB-4D53-EE49-B415-1CC7E00333E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1120" yWindow="2000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -852,7 +852,7 @@
     <t>XYZ1</t>
   </si>
   <si>
-    <t>fcs</t>
+    <t>vericell.fcs</t>
   </si>
 </sst>
 </file>
@@ -979,11 +979,11 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1326,7 +1326,7 @@
   <dimension ref="A1:P211"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1339,23 +1339,23 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1526,25 +1526,25 @@
       <c r="P8" s="2"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2720,17 +2720,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -2768,31 +2768,31 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <v>3983272</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2800,31 +2800,31 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <v>1231272</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="5" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated CyTOF metadata template (#275)
* move batch_id to preamble section

* normalized & debarcoded fcs filename

* add file desc

* added Spike-in FCS file to preamble

* bump __version__ = 0.14.8

* update docs

* update property desc
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C6B77A-D6A8-8F43-9B11-D870F0304011}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89596AB-4D53-EE49-B415-1CC7E00333E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1120" yWindow="2000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
     <sheet name="Antibody Information" sheetId="2" r:id="rId2"/>
+    <sheet name="Legend" sheetId="3" r:id="rId3"/>
+    <sheet name="Data Dictionary" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -31,7 +33,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -91,7 +93,53 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Path to a file on a User's computer. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This file contains the normalized &amp; debarcoded spike-in for a batch.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CyTOF batch identification number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -113,11 +161,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>CyTOF batch identification number.</t>
+          <t>Path to a file on a user's computer.
+In .fcs format</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -126,11 +175,13 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.</t>
+          <t>Path to a file on a User's computer. 
+This .fcs file has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
+In .fcs format</t>
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -143,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -156,7 +207,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -169,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -182,7 +233,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -195,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -204,11 +255,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.</t>
+          <t>Path to a file on a user's computer.
+In .fcs format</t>
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +286,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -247,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="N11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -260,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="O11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -273,7 +325,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="P11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -418,7 +470,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="127">
   <si>
     <t>#t</t>
   </si>
@@ -444,6 +496,12 @@
     <t>Instrument</t>
   </si>
   <si>
+    <t>Spike in fcs filename</t>
+  </si>
+  <si>
+    <t>Batch id</t>
+  </si>
+  <si>
     <t>Run info</t>
   </si>
   <si>
@@ -459,10 +517,10 @@
     <t>Cimac id</t>
   </si>
   <si>
-    <t>Batch_id</t>
-  </si>
-  <si>
-    <t>Original fcs filename(s)</t>
+    <t>Raw fcs filename(s)</t>
+  </si>
+  <si>
+    <t>Normalized &amp; debarcoded fcs filename</t>
   </si>
   <si>
     <t>Date of acquisition</t>
@@ -531,116 +589,277 @@
     <t>Usage</t>
   </si>
   <si>
+    <t>LEGEND</t>
+  </si>
+  <si>
+    <t>Legend for tab 'Acquisition and Preprocessing'</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>User defined unique identifier for this assay run.</t>
+  </si>
+  <si>
+    <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <t>Indicates what site is filling out the assay.</t>
+  </si>
+  <si>
+    <t>E.g. 'DFCI'</t>
+  </si>
+  <si>
+    <t>Standardized CyTOF panel name used for antibody sample development.</t>
+  </si>
+  <si>
+    <t>Name of CyTOF instrument on which experiment was conducted.</t>
+  </si>
+  <si>
+    <t>Path to a file on a User's computer. 
+This file contains the normalized &amp; debarcoded spike-in for a batch.</t>
+  </si>
+  <si>
+    <t>CyTOF batch identification number.</t>
+  </si>
+  <si>
+    <t>Section 'Run info' of tab 'Acquisition and Preprocessing'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">String: regex ^C[A-Z0-9]{3}[A-Z0-9]{3}[A-Z0-9]{2}.[0-9]{2}$ </t>
+  </si>
+  <si>
+    <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+  </si>
+  <si>
+    <t>E.g. 'CTTTP01A1.00'</t>
+  </si>
+  <si>
+    <t>Path to a file on a user's computer.</t>
+  </si>
+  <si>
+    <t>Path to a file on a User's computer. 
+This .fcs file has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.</t>
+  </si>
+  <si>
+    <t>Date of CyTOF batch acquisition.</t>
+  </si>
+  <si>
+    <t>Name of Injector component used as part of the CyTOF software</t>
+  </si>
+  <si>
+    <t>Cell staining buffer used for antibody and cell dilution.</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Analysis rate of CyTOF expressions per second.</t>
+  </si>
+  <si>
+    <t>Length of run time for CyTOF experiment.</t>
+  </si>
+  <si>
+    <t>Section 'Preprocessing' of tab 'Acquisition and Preprocessing'</t>
+  </si>
+  <si>
+    <t>Concatenation of FCS files into a single FCS version number.</t>
+  </si>
+  <si>
+    <t>Version of normalization for CyTOF assay batch.</t>
+  </si>
+  <si>
+    <t>Confirmation of beads being removed after normalization process.</t>
+  </si>
+  <si>
+    <t>E.g. 'Y'</t>
+  </si>
+  <si>
+    <t>Protocol for the download and installation of the Debarcoder CyTOF software feature.</t>
+  </si>
+  <si>
+    <t>Key required for access to the Debarcoding software.</t>
+  </si>
+  <si>
+    <t>Any notes pertaining to preprocessing of CyTOF data.</t>
+  </si>
+  <si>
+    <t>Legend for tab 'Antibody Information'</t>
+  </si>
+  <si>
+    <t>Section 'Samples' of tab 'Antibody Information'</t>
+  </si>
+  <si>
+    <t>Antibody type collected for this study.</t>
+  </si>
+  <si>
+    <t>Resulting type of antibody clone from primary antibody sample.</t>
+  </si>
+  <si>
+    <t>Company from which antibody sample was derived.</t>
+  </si>
+  <si>
+    <t>Antibody registry catalog number assigned to antibody sample.</t>
+  </si>
+  <si>
+    <t>Identification number assigned to the particular quantity or lot of material from manufacturer.</t>
+  </si>
+  <si>
+    <t>Antibody isotype used to help differentiate antibody signals.</t>
+  </si>
+  <si>
+    <t>Concentration ratio of dilution buffer for primary antibody.</t>
+  </si>
+  <si>
+    <t>Type of staining method used for antibody.</t>
+  </si>
+  <si>
+    <t>E.g. 'Surface Stain'</t>
+  </si>
+  <si>
+    <t>How this antibody should be used in automatic analysis</t>
+  </si>
+  <si>
+    <t>E.g. 'Ignored'</t>
+  </si>
+  <si>
     <t>DFCI</t>
   </si>
   <si>
+    <t>Mount Sinai</t>
+  </si>
+  <si>
+    <t>Stanford</t>
+  </si>
+  <si>
+    <t>MD Anderson</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Surface Stain</t>
+  </si>
+  <si>
+    <t>Intracellular</t>
+  </si>
+  <si>
+    <t>Ignored</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>Analysis Only</t>
+  </si>
+  <si>
+    <t>CD8</t>
+  </si>
+  <si>
+    <t>C8/144b</t>
+  </si>
+  <si>
+    <t>DAKO</t>
+  </si>
+  <si>
+    <t>C8-ABC</t>
+  </si>
+  <si>
+    <t>146Nd</t>
+  </si>
+  <si>
+    <t>100X</t>
+  </si>
+  <si>
+    <t>PD-L1</t>
+  </si>
+  <si>
+    <t>C2/11p</t>
+  </si>
+  <si>
+    <t>C8-AB123</t>
+  </si>
+  <si>
+    <t>146Nb</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>sample1a.fcs,sample1b.fcs</t>
+  </si>
+  <si>
+    <t>sample1_n.fcs</t>
+  </si>
+  <si>
+    <t>HAT123</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>sample1.fcs</t>
+  </si>
+  <si>
+    <t>GHIL</t>
+  </si>
+  <si>
+    <t>FLUIDIGM XYZ</t>
+  </si>
+  <si>
+    <t>FLUIDIGM 1234</t>
+  </si>
+  <si>
+    <t>a note like any other note</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>sample2a.fcs,sample2b.fcs</t>
+  </si>
+  <si>
+    <t>sample2_n.fcs</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>sample2.fcs</t>
+  </si>
+  <si>
+    <t>a different note</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id_run_1</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
     <t>IMMUNE4</t>
   </si>
   <si>
     <t>PresNixon123</t>
   </si>
   <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
     <t>XYZ1</t>
   </si>
   <si>
-    <t>sample1a.fcs,sample1b.fcs</t>
-  </si>
-  <si>
-    <t>HAT123</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>sample1.fcs</t>
-  </si>
-  <si>
-    <t>GHIL</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>FLUIDIGM XYZ</t>
-  </si>
-  <si>
-    <t>FLUIDIGM 1234</t>
-  </si>
-  <si>
-    <t>a note like any other note</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2a.fcs,sample2b.fcs</t>
-  </si>
-  <si>
-    <t>ABCD</t>
-  </si>
-  <si>
-    <t>sample2.fcs</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>a different note</t>
-  </si>
-  <si>
-    <t>CD8</t>
-  </si>
-  <si>
-    <t>C8/144b</t>
-  </si>
-  <si>
-    <t>DAKO</t>
-  </si>
-  <si>
-    <t>C8-ABC</t>
-  </si>
-  <si>
-    <t>146Nd</t>
-  </si>
-  <si>
-    <t>100X</t>
-  </si>
-  <si>
-    <t>Surface Stain</t>
-  </si>
-  <si>
-    <t>Used</t>
-  </si>
-  <si>
-    <t>PD-L1</t>
-  </si>
-  <si>
-    <t>C2/11p</t>
-  </si>
-  <si>
-    <t>C8-AB123</t>
-  </si>
-  <si>
-    <t>146Nb</t>
-  </si>
-  <si>
-    <t>Analysis Only</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id_run_1</t>
+    <t>vericell.fcs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,13 +882,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -678,8 +890,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -710,12 +922,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB2D2F6"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor rgb="FF5FA3F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -749,35 +961,25 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFFFFFFF"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1121,10 +1323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P209"/>
+  <dimension ref="A1:P211"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1133,1317 +1335,1368 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
     </row>
     <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="C2" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="C3" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
     </row>
     <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="C4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
     </row>
     <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="C5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
     </row>
     <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B8" s="7" t="s">
+      <c r="C6" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+    </row>
+    <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C8" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10">
-        <v>43355</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10">
-        <v>123</v>
-      </c>
-      <c r="I10">
-        <v>23</v>
-      </c>
-      <c r="J10" t="s">
-        <v>45</v>
-      </c>
-      <c r="K10" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M10" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" t="s">
-        <v>48</v>
-      </c>
-      <c r="O10" t="s">
-        <v>49</v>
-      </c>
-      <c r="P10" t="s">
-        <v>50</v>
-      </c>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11">
-        <v>43385</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11">
-        <v>123</v>
-      </c>
-      <c r="I11">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="J11" t="s">
-        <v>54</v>
-      </c>
-      <c r="K11" t="s">
-        <v>46</v>
-      </c>
-      <c r="L11" t="s">
-        <v>44</v>
-      </c>
-      <c r="M11" t="s">
-        <v>55</v>
-      </c>
-      <c r="N11" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E12">
+        <v>43355</v>
+      </c>
+      <c r="F12" t="s">
+        <v>108</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12">
+        <v>123</v>
+      </c>
+      <c r="I12">
+        <v>23</v>
+      </c>
+      <c r="J12" t="s">
+        <v>110</v>
+      </c>
+      <c r="K12" t="s">
+        <v>111</v>
+      </c>
+      <c r="L12" t="s">
+        <v>109</v>
+      </c>
+      <c r="M12" t="s">
+        <v>88</v>
+      </c>
+      <c r="N12" t="s">
+        <v>112</v>
+      </c>
+      <c r="O12" t="s">
+        <v>113</v>
+      </c>
+      <c r="P12" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13" t="s">
+        <v>117</v>
+      </c>
+      <c r="E13">
+        <v>43385</v>
+      </c>
+      <c r="F13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13">
+        <v>123</v>
+      </c>
+      <c r="I13">
+        <v>28</v>
+      </c>
+      <c r="J13" t="s">
+        <v>119</v>
+      </c>
+      <c r="K13" t="s">
+        <v>111</v>
+      </c>
+      <c r="L13" t="s">
+        <v>109</v>
+      </c>
+      <c r="M13" t="s">
+        <v>89</v>
+      </c>
+      <c r="N13" t="s">
+        <v>112</v>
+      </c>
+      <c r="O13" t="s">
+        <v>113</v>
+      </c>
+      <c r="P13" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="J8:P8"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="J10:P10"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M10:M209" xr:uid="{00000000-0002-0000-0000-000001000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:M211" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2457,7 +2710,7 @@
   <dimension ref="A1:J202"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B3" sqref="B3:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2467,1102 +2720,1102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="H2" s="3" t="s">
         <v>36</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F3" s="6">
+        <v>13</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="5">
         <v>3983272</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>64</v>
+      <c r="G3" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F4" s="6">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="5">
         <v>1231272</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>69</v>
+      <c r="G4" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -3570,14 +3823,489 @@
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Surface Stain,Intracellular"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J202" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Ignored,Used,Analysis Only"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:E37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>44</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+      <c r="E36" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="B1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="101" width="30.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Move source FCS file(s) up to batch level
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89596AB-4D53-EE49-B415-1CC7E00333E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8627821-CBDE-9B46-A654-A1EADFDFE659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="2000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22340" yWindow="640" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -98,61 +98,17 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Path to a file on a User's computer. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This file contains the normalized &amp; debarcoded spike-in for a batch.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In .fcs format</t>
+          <t>Path to a file on a User's computer. 
+This file contains the normalized &amp; debarcoded spike-in for a batch.
+In .fcs format</t>
         </r>
       </text>
     </comment>
     <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CyTOF batch identification number.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -166,7 +122,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CyTOF batch identification number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -194,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -207,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -220,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -233,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -246,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -260,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -273,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="K12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="L12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -299,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="M12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -308,11 +290,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Protocol for the download and installation of the Debarcoder CyTOF software feature.</t>
+          <t>The strategy/kit used to barcode CyTOF samples.</t>
         </r>
       </text>
     </comment>
-    <comment ref="O11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="N12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -321,11 +303,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Key required for access to the Debarcoding software.</t>
+          <t>An ID that maps to the specific isotope labeling scheme in the debarcoding protocol.</t>
         </r>
       </text>
     </comment>
-    <comment ref="P11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -470,7 +452,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="126">
   <si>
     <t>#t</t>
   </si>
@@ -499,6 +481,9 @@
     <t>Spike in fcs filename</t>
   </si>
   <si>
+    <t>Raw fcs filename(s)</t>
+  </si>
+  <si>
     <t>Batch id</t>
   </si>
   <si>
@@ -515,9 +500,6 @@
   </si>
   <si>
     <t>Cimac id</t>
-  </si>
-  <si>
-    <t>Raw fcs filename(s)</t>
   </si>
   <si>
     <t>Normalized &amp; debarcoded fcs filename</t>
@@ -623,6 +605,9 @@
 This file contains the normalized &amp; debarcoded spike-in for a batch.</t>
   </si>
   <si>
+    <t>Path to a file on a user's computer.</t>
+  </si>
+  <si>
     <t>CyTOF batch identification number.</t>
   </si>
   <si>
@@ -636,9 +621,6 @@
   </si>
   <si>
     <t>E.g. 'CTTTP01A1.00'</t>
-  </si>
-  <si>
-    <t>Path to a file on a user's computer.</t>
   </si>
   <si>
     <t>Path to a file on a User's computer. 
@@ -678,10 +660,10 @@
     <t>E.g. 'Y'</t>
   </si>
   <si>
-    <t>Protocol for the download and installation of the Debarcoder CyTOF software feature.</t>
-  </si>
-  <si>
-    <t>Key required for access to the Debarcoding software.</t>
+    <t>The strategy/kit used to barcode CyTOF samples.</t>
+  </si>
+  <si>
+    <t>An ID that maps to the specific isotope labeling scheme in the debarcoding protocol.</t>
   </si>
   <si>
     <t>Any notes pertaining to preprocessing of CyTOF data.</t>
@@ -759,6 +741,69 @@
     <t>Analysis Only</t>
   </si>
   <si>
+    <t>test_prism_trial_id_run_1</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>IMMUNE4</t>
+  </si>
+  <si>
+    <t>PresNixon123</t>
+  </si>
+  <si>
+    <t>vericell.fcs</t>
+  </si>
+  <si>
+    <t>batch1f1.fcs,batch1f2.fcs</t>
+  </si>
+  <si>
+    <t>XYZ1</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>sample1_n.fcs</t>
+  </si>
+  <si>
+    <t>HAT123</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>sample1.fcs</t>
+  </si>
+  <si>
+    <t>GHIL</t>
+  </si>
+  <si>
+    <t>FLUIDIGM XYZ</t>
+  </si>
+  <si>
+    <t>FLUIDIGM 1234</t>
+  </si>
+  <si>
+    <t>a note like any other note</t>
+  </si>
+  <si>
+    <t>sample2_n.fcs</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>sample2.fcs</t>
+  </si>
+  <si>
+    <t>a different note</t>
+  </si>
+  <si>
     <t>CD8</t>
   </si>
   <si>
@@ -787,79 +832,13 @@
   </si>
   <si>
     <t>146Nb</t>
-  </si>
-  <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>sample1a.fcs,sample1b.fcs</t>
-  </si>
-  <si>
-    <t>sample1_n.fcs</t>
-  </si>
-  <si>
-    <t>HAT123</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>sample1.fcs</t>
-  </si>
-  <si>
-    <t>GHIL</t>
-  </si>
-  <si>
-    <t>FLUIDIGM XYZ</t>
-  </si>
-  <si>
-    <t>FLUIDIGM 1234</t>
-  </si>
-  <si>
-    <t>a note like any other note</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2a.fcs,sample2b.fcs</t>
-  </si>
-  <si>
-    <t>sample2_n.fcs</t>
-  </si>
-  <si>
-    <t>ABCD</t>
-  </si>
-  <si>
-    <t>sample2.fcs</t>
-  </si>
-  <si>
-    <t>a different note</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id_run_1</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>IMMUNE4</t>
-  </si>
-  <si>
-    <t>PresNixon123</t>
-  </si>
-  <si>
-    <t>XYZ1</t>
-  </si>
-  <si>
-    <t>vericell.fcs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,19 +857,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -965,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -978,9 +944,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1323,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P211"/>
+  <dimension ref="A1:O212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="B6" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1335,29 +1298,28 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1327,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1379,9 +1341,8 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1389,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1403,9 +1364,8 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1427,9 +1387,8 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1437,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1451,9 +1410,8 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1461,7 +1419,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1475,9 +1433,8 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1485,7 +1442,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1499,9 +1456,8 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1509,7 +1465,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1523,1180 +1479,1192 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+    </row>
+    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6" t="s">
+      <c r="C9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13">
+        <v>43355</v>
+      </c>
+      <c r="E13" t="s">
         <v>105</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F13" t="s">
         <v>106</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G13">
+        <v>123</v>
+      </c>
+      <c r="H13">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
         <v>107</v>
       </c>
-      <c r="E12">
-        <v>43355</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="J13" t="s">
         <v>108</v>
       </c>
-      <c r="G12" t="s">
+      <c r="K13" t="s">
+        <v>106</v>
+      </c>
+      <c r="L13" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" t="s">
         <v>109</v>
       </c>
-      <c r="H12">
+      <c r="N13" t="s">
+        <v>110</v>
+      </c>
+      <c r="O13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14">
+        <v>43385</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14">
         <v>123</v>
       </c>
-      <c r="I12">
-        <v>23</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="H14">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" t="s">
+        <v>108</v>
+      </c>
+      <c r="K14" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" t="s">
+        <v>109</v>
+      </c>
+      <c r="N14" t="s">
         <v>110</v>
       </c>
-      <c r="K12" t="s">
-        <v>111</v>
-      </c>
-      <c r="L12" t="s">
-        <v>109</v>
-      </c>
-      <c r="M12" t="s">
-        <v>88</v>
-      </c>
-      <c r="N12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O12" t="s">
-        <v>113</v>
-      </c>
-      <c r="P12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="O14" t="s">
         <v>115</v>
       </c>
-      <c r="C13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13">
-        <v>43385</v>
-      </c>
-      <c r="F13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H13">
-        <v>123</v>
-      </c>
-      <c r="I13">
-        <v>28</v>
-      </c>
-      <c r="J13" t="s">
-        <v>119</v>
-      </c>
-      <c r="K13" t="s">
-        <v>111</v>
-      </c>
-      <c r="L13" t="s">
-        <v>109</v>
-      </c>
-      <c r="M13" t="s">
-        <v>89</v>
-      </c>
-      <c r="N13" t="s">
-        <v>112</v>
-      </c>
-      <c r="O13" t="s">
-        <v>113</v>
-      </c>
-      <c r="P13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="J10:P10"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="I11:O11"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{55F3624C-F6BC-154A-8466-26A26F07AC3E}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:M211" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:L212" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2709,7 +2677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:J4"/>
     </sheetView>
   </sheetViews>
@@ -2720,21 +2688,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>30</v>
@@ -2766,1056 +2734,1056 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="5">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3">
         <v>3983272</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="G3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="5">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4">
         <v>1231272</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="G4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3936,23 +3904,20 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="11" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -3960,9 +3925,12 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4045,7 +4013,7 @@
         <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
CyTOF raw fcs data model fix (#277)
* Move source FCS file(s) up to batch level

* Bump package version

* Update tests to reflect new CyTOF schema
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B89596AB-4D53-EE49-B415-1CC7E00333E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8627821-CBDE-9B46-A654-A1EADFDFE659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="2000" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22340" yWindow="640" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -98,61 +98,17 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Path to a file on a User's computer. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This file contains the normalized &amp; debarcoded spike-in for a batch.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In .fcs format</t>
+          <t>Path to a file on a User's computer. 
+This file contains the normalized &amp; debarcoded spike-in for a batch.
+In .fcs format</t>
         </r>
       </text>
     </comment>
     <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>CyTOF batch identification number.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -166,7 +122,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CyTOF batch identification number.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -181,7 +163,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -194,7 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -207,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -220,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -233,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -246,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -260,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -273,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="K12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="L12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -299,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="M12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -308,11 +290,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Protocol for the download and installation of the Debarcoder CyTOF software feature.</t>
+          <t>The strategy/kit used to barcode CyTOF samples.</t>
         </r>
       </text>
     </comment>
-    <comment ref="O11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
+    <comment ref="N12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -321,11 +303,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Key required for access to the Debarcoding software.</t>
+          <t>An ID that maps to the specific isotope labeling scheme in the debarcoding protocol.</t>
         </r>
       </text>
     </comment>
-    <comment ref="P11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
+    <comment ref="O12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -470,7 +452,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="126">
   <si>
     <t>#t</t>
   </si>
@@ -499,6 +481,9 @@
     <t>Spike in fcs filename</t>
   </si>
   <si>
+    <t>Raw fcs filename(s)</t>
+  </si>
+  <si>
     <t>Batch id</t>
   </si>
   <si>
@@ -515,9 +500,6 @@
   </si>
   <si>
     <t>Cimac id</t>
-  </si>
-  <si>
-    <t>Raw fcs filename(s)</t>
   </si>
   <si>
     <t>Normalized &amp; debarcoded fcs filename</t>
@@ -623,6 +605,9 @@
 This file contains the normalized &amp; debarcoded spike-in for a batch.</t>
   </si>
   <si>
+    <t>Path to a file on a user's computer.</t>
+  </si>
+  <si>
     <t>CyTOF batch identification number.</t>
   </si>
   <si>
@@ -636,9 +621,6 @@
   </si>
   <si>
     <t>E.g. 'CTTTP01A1.00'</t>
-  </si>
-  <si>
-    <t>Path to a file on a user's computer.</t>
   </si>
   <si>
     <t>Path to a file on a User's computer. 
@@ -678,10 +660,10 @@
     <t>E.g. 'Y'</t>
   </si>
   <si>
-    <t>Protocol for the download and installation of the Debarcoder CyTOF software feature.</t>
-  </si>
-  <si>
-    <t>Key required for access to the Debarcoding software.</t>
+    <t>The strategy/kit used to barcode CyTOF samples.</t>
+  </si>
+  <si>
+    <t>An ID that maps to the specific isotope labeling scheme in the debarcoding protocol.</t>
   </si>
   <si>
     <t>Any notes pertaining to preprocessing of CyTOF data.</t>
@@ -759,6 +741,69 @@
     <t>Analysis Only</t>
   </si>
   <si>
+    <t>test_prism_trial_id_run_1</t>
+  </si>
+  <si>
+    <t>test_prism_trial_id</t>
+  </si>
+  <si>
+    <t>IMMUNE4</t>
+  </si>
+  <si>
+    <t>PresNixon123</t>
+  </si>
+  <si>
+    <t>vericell.fcs</t>
+  </si>
+  <si>
+    <t>batch1f1.fcs,batch1f2.fcs</t>
+  </si>
+  <si>
+    <t>XYZ1</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>sample1_n.fcs</t>
+  </si>
+  <si>
+    <t>HAT123</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>sample1.fcs</t>
+  </si>
+  <si>
+    <t>GHIL</t>
+  </si>
+  <si>
+    <t>FLUIDIGM XYZ</t>
+  </si>
+  <si>
+    <t>FLUIDIGM 1234</t>
+  </si>
+  <si>
+    <t>a note like any other note</t>
+  </si>
+  <si>
+    <t>sample2_n.fcs</t>
+  </si>
+  <si>
+    <t>ABCD</t>
+  </si>
+  <si>
+    <t>sample2.fcs</t>
+  </si>
+  <si>
+    <t>a different note</t>
+  </si>
+  <si>
     <t>CD8</t>
   </si>
   <si>
@@ -787,79 +832,13 @@
   </si>
   <si>
     <t>146Nb</t>
-  </si>
-  <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>sample1a.fcs,sample1b.fcs</t>
-  </si>
-  <si>
-    <t>sample1_n.fcs</t>
-  </si>
-  <si>
-    <t>HAT123</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>sample1.fcs</t>
-  </si>
-  <si>
-    <t>GHIL</t>
-  </si>
-  <si>
-    <t>FLUIDIGM XYZ</t>
-  </si>
-  <si>
-    <t>FLUIDIGM 1234</t>
-  </si>
-  <si>
-    <t>a note like any other note</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2a.fcs,sample2b.fcs</t>
-  </si>
-  <si>
-    <t>sample2_n.fcs</t>
-  </si>
-  <si>
-    <t>ABCD</t>
-  </si>
-  <si>
-    <t>sample2.fcs</t>
-  </si>
-  <si>
-    <t>a different note</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id_run_1</t>
-  </si>
-  <si>
-    <t>test_prism_trial_id</t>
-  </si>
-  <si>
-    <t>IMMUNE4</t>
-  </si>
-  <si>
-    <t>PresNixon123</t>
-  </si>
-  <si>
-    <t>XYZ1</t>
-  </si>
-  <si>
-    <t>vericell.fcs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -878,19 +857,6 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -965,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -978,9 +944,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1323,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P211"/>
+  <dimension ref="A1:O212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView topLeftCell="B6" zoomScale="75" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1335,29 +1298,28 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1327,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>121</v>
+        <v>95</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -1379,9 +1341,8 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1389,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>122</v>
+        <v>96</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -1403,9 +1364,8 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1427,9 +1387,8 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1437,7 +1396,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>123</v>
+        <v>97</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1451,9 +1410,8 @@
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-    </row>
-    <row r="6" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1461,7 +1419,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>124</v>
+        <v>98</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1475,9 +1433,8 @@
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-    </row>
-    <row r="7" spans="1:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1485,7 +1442,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -1499,9 +1456,8 @@
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-    </row>
-    <row r="8" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1509,7 +1465,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1523,1180 +1479,1192 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="B10" s="6" t="s">
+    </row>
+    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6" t="s">
+      <c r="C9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N11" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="O11" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="P11" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13">
+        <v>43355</v>
+      </c>
+      <c r="E13" t="s">
         <v>105</v>
       </c>
-      <c r="C12" t="s">
+      <c r="F13" t="s">
         <v>106</v>
       </c>
-      <c r="D12" t="s">
+      <c r="G13">
+        <v>123</v>
+      </c>
+      <c r="H13">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
         <v>107</v>
       </c>
-      <c r="E12">
-        <v>43355</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="J13" t="s">
         <v>108</v>
       </c>
-      <c r="G12" t="s">
+      <c r="K13" t="s">
+        <v>106</v>
+      </c>
+      <c r="L13" t="s">
+        <v>88</v>
+      </c>
+      <c r="M13" t="s">
         <v>109</v>
       </c>
-      <c r="H12">
+      <c r="N13" t="s">
+        <v>110</v>
+      </c>
+      <c r="O13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C14" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14">
+        <v>43385</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14">
         <v>123</v>
       </c>
-      <c r="I12">
-        <v>23</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="H14">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>114</v>
+      </c>
+      <c r="J14" t="s">
+        <v>108</v>
+      </c>
+      <c r="K14" t="s">
+        <v>106</v>
+      </c>
+      <c r="L14" t="s">
+        <v>89</v>
+      </c>
+      <c r="M14" t="s">
+        <v>109</v>
+      </c>
+      <c r="N14" t="s">
         <v>110</v>
       </c>
-      <c r="K12" t="s">
-        <v>111</v>
-      </c>
-      <c r="L12" t="s">
-        <v>109</v>
-      </c>
-      <c r="M12" t="s">
-        <v>88</v>
-      </c>
-      <c r="N12" t="s">
-        <v>112</v>
-      </c>
-      <c r="O12" t="s">
-        <v>113</v>
-      </c>
-      <c r="P12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="O14" t="s">
         <v>115</v>
       </c>
-      <c r="C13" t="s">
-        <v>116</v>
-      </c>
-      <c r="D13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13">
-        <v>43385</v>
-      </c>
-      <c r="F13" t="s">
-        <v>108</v>
-      </c>
-      <c r="G13" t="s">
-        <v>118</v>
-      </c>
-      <c r="H13">
-        <v>123</v>
-      </c>
-      <c r="I13">
-        <v>28</v>
-      </c>
-      <c r="J13" t="s">
-        <v>119</v>
-      </c>
-      <c r="K13" t="s">
-        <v>111</v>
-      </c>
-      <c r="L13" t="s">
-        <v>109</v>
-      </c>
-      <c r="M13" t="s">
-        <v>89</v>
-      </c>
-      <c r="N13" t="s">
-        <v>112</v>
-      </c>
-      <c r="O13" t="s">
-        <v>113</v>
-      </c>
-      <c r="P13" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="J10:P10"/>
+    <mergeCell ref="B1:O1"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="I11:O11"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{55F3624C-F6BC-154A-8466-26A26F07AC3E}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M12:M211" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:L212" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2709,7 +2677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J202"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3:J4"/>
     </sheetView>
   </sheetViews>
@@ -2720,21 +2688,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>30</v>
@@ -2766,1056 +2734,1056 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="5">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F3">
         <v>3983272</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I3" s="5" t="s">
+      <c r="G3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" t="s">
         <v>90</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F4" s="5">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4">
         <v>1231272</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="G4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -3936,23 +3904,20 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="11" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
@@ -3960,9 +3925,12 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4045,7 +4013,7 @@
         <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
spike-in fcs filename: optional
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8627821-CBDE-9B46-A654-A1EADFDFE659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0FE4BE-DD94-C94A-A2A9-2F0994FBF5B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22340" yWindow="640" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -452,7 +452,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="125">
   <si>
     <t>#t</t>
   </si>
@@ -753,9 +753,6 @@
     <t>PresNixon123</t>
   </si>
   <si>
-    <t>vericell.fcs</t>
-  </si>
-  <si>
     <t>batch1f1.fcs,batch1f2.fcs</t>
   </si>
   <si>
@@ -765,31 +762,31 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
+    <t>sample1_n.fcs</t>
+  </si>
+  <si>
+    <t>HAT123</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>sample1.fcs</t>
+  </si>
+  <si>
+    <t>GHIL</t>
+  </si>
+  <si>
+    <t>FLUIDIGM XYZ</t>
+  </si>
+  <si>
+    <t>FLUIDIGM 1234</t>
+  </si>
+  <si>
+    <t>a note like any other note</t>
+  </si>
+  <si>
     <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample1_n.fcs</t>
-  </si>
-  <si>
-    <t>HAT123</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>sample1.fcs</t>
-  </si>
-  <si>
-    <t>GHIL</t>
-  </si>
-  <si>
-    <t>FLUIDIGM XYZ</t>
-  </si>
-  <si>
-    <t>FLUIDIGM 1234</t>
-  </si>
-  <si>
-    <t>a note like any other note</t>
   </si>
   <si>
     <t>sample2_n.fcs</t>
@@ -838,7 +835,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,6 +854,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1288,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O212"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:O14"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1298,7 +1301,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1322,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1342,7 +1345,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1368,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1388,7 +1391,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1414,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1434,16 +1437,14 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1457,7 +1458,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1480,7 +1481,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1575,19 +1576,19 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
         <v>102</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
       </c>
       <c r="D13">
         <v>43355</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G13">
         <v>123</v>
@@ -1596,25 +1597,25 @@
         <v>23</v>
       </c>
       <c r="I13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L13" t="s">
         <v>88</v>
       </c>
       <c r="M13" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" t="s">
         <v>109</v>
-      </c>
-      <c r="N13" t="s">
-        <v>110</v>
-      </c>
-      <c r="O13" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1622,19 +1623,19 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14">
         <v>43385</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G14">
         <v>123</v>
@@ -1643,25 +1644,25 @@
         <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L14" t="s">
         <v>89</v>
       </c>
       <c r="M14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -2660,8 +2661,8 @@
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="I11:O11"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{55F3624C-F6BC-154A-8466-26A26F07AC3E}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:L212" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -2678,7 +2679,7 @@
   <dimension ref="A1:J202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2737,25 +2738,25 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
         <v>116</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>117</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>118</v>
-      </c>
-      <c r="E3" t="s">
-        <v>119</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
         <v>120</v>
-      </c>
-      <c r="H3" t="s">
-        <v>121</v>
       </c>
       <c r="I3" t="s">
         <v>90</v>
@@ -2769,25 +2770,25 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
         <v>122</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
         <v>123</v>
-      </c>
-      <c r="D4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>124</v>
       </c>
       <c r="F4">
         <v>1231272</v>
       </c>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
         <v>90</v>
@@ -3790,11 +3791,11 @@
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Surface Stain,Intracellular"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J202" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Ignored,Used,Analysis Only"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
spike-in FCS filename: optional (#282)
* spike-in fcs filename: optional

* bump __version__ = '0.15.6'
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/template_examples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/PycharmProjects/schema/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8627821-CBDE-9B46-A654-A1EADFDFE659}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D0FE4BE-DD94-C94A-A2A9-2F0994FBF5B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22340" yWindow="640" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -452,7 +452,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="125">
   <si>
     <t>#t</t>
   </si>
@@ -753,9 +753,6 @@
     <t>PresNixon123</t>
   </si>
   <si>
-    <t>vericell.fcs</t>
-  </si>
-  <si>
     <t>batch1f1.fcs,batch1f2.fcs</t>
   </si>
   <si>
@@ -765,31 +762,31 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
+    <t>sample1_n.fcs</t>
+  </si>
+  <si>
+    <t>HAT123</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>sample1.fcs</t>
+  </si>
+  <si>
+    <t>GHIL</t>
+  </si>
+  <si>
+    <t>FLUIDIGM XYZ</t>
+  </si>
+  <si>
+    <t>FLUIDIGM 1234</t>
+  </si>
+  <si>
+    <t>a note like any other note</t>
+  </si>
+  <si>
     <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample1_n.fcs</t>
-  </si>
-  <si>
-    <t>HAT123</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>sample1.fcs</t>
-  </si>
-  <si>
-    <t>GHIL</t>
-  </si>
-  <si>
-    <t>FLUIDIGM XYZ</t>
-  </si>
-  <si>
-    <t>FLUIDIGM 1234</t>
-  </si>
-  <si>
-    <t>a note like any other note</t>
   </si>
   <si>
     <t>sample2_n.fcs</t>
@@ -838,7 +835,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -857,6 +854,12 @@
     <font>
       <sz val="10"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -1288,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O212"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:O14"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1298,7 +1301,7 @@
     <col min="2" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1322,7 @@
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1342,7 +1345,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1368,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1388,7 +1391,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1411,7 +1414,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
     </row>
-    <row r="6" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1434,16 +1437,14 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>99</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
@@ -1457,7 +1458,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -1480,7 +1481,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -1575,19 +1576,19 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
         <v>102</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
       </c>
       <c r="D13">
         <v>43355</v>
       </c>
       <c r="E13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G13">
         <v>123</v>
@@ -1596,25 +1597,25 @@
         <v>23</v>
       </c>
       <c r="I13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="J13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L13" t="s">
         <v>88</v>
       </c>
       <c r="M13" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" t="s">
+        <v>108</v>
+      </c>
+      <c r="O13" t="s">
         <v>109</v>
-      </c>
-      <c r="N13" t="s">
-        <v>110</v>
-      </c>
-      <c r="O13" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -1622,19 +1623,19 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D14">
         <v>43385</v>
       </c>
       <c r="E14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G14">
         <v>123</v>
@@ -1643,25 +1644,25 @@
         <v>28</v>
       </c>
       <c r="I14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L14" t="s">
         <v>89</v>
       </c>
       <c r="M14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="N14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
@@ -2660,8 +2661,8 @@
     <mergeCell ref="B11:H11"/>
     <mergeCell ref="I11:O11"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{55F3624C-F6BC-154A-8466-26A26F07AC3E}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:L212" xr:uid="{00000000-0002-0000-0000-000001000000}">
@@ -2678,7 +2679,7 @@
   <dimension ref="A1:J202"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:J4"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2737,25 +2738,25 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
         <v>116</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>117</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>118</v>
-      </c>
-      <c r="E3" t="s">
-        <v>119</v>
       </c>
       <c r="F3">
         <v>3983272</v>
       </c>
       <c r="G3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3" t="s">
         <v>120</v>
-      </c>
-      <c r="H3" t="s">
-        <v>121</v>
       </c>
       <c r="I3" t="s">
         <v>90</v>
@@ -2769,25 +2770,25 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
         <v>122</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
         <v>123</v>
-      </c>
-      <c r="D4" t="s">
-        <v>118</v>
-      </c>
-      <c r="E4" t="s">
-        <v>124</v>
       </c>
       <c r="F4">
         <v>1231272</v>
       </c>
       <c r="G4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I4" t="s">
         <v>90</v>
@@ -3790,11 +3791,11 @@
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Surface Stain,Intracellular"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J202" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Ignored,Used,Analysis Only"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
rename normalized_debarcoded_fcs -> intermediate_fcs
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB67DFD6-CB47-5447-B69E-AB8B296ADA44}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B282D47-0481-1B4D-922F-6EF9B4E40D1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10560" yWindow="2800" windowWidth="16100" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
             <family val="2"/>
           </rPr>
           <t>Path to a file on a User's computer. 
-This .fcs file has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
+This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
 In .fcs format</t>
         </r>
       </text>
@@ -507,11 +507,11 @@
     <t>E.g. 'CTTTP01A1.00'</t>
   </si>
   <si>
-    <t>Normalized &amp; debarcoded fcs filename</t>
+    <t>Intermediate fcs filename</t>
   </si>
   <si>
     <t>Path to a file on a User's computer. 
-This .fcs file has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.</t>
+This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.</t>
   </si>
   <si>
     <t>Date of acquisition</t>
@@ -733,15 +733,6 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2_n.fcs</t>
-  </si>
-  <si>
-    <t>ABCD</t>
-  </si>
-  <si>
     <t>sample1.fcs</t>
   </si>
   <si>
@@ -755,6 +746,15 @@
   </si>
   <si>
     <t>a note like any other note</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>sample2_n.fcs</t>
+  </si>
+  <si>
+    <t>ABCD</t>
   </si>
   <si>
     <t>sample2.fcs</t>
@@ -1247,8 +1247,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2012"/>
   <sheetViews>
-    <sheetView topLeftCell="J3" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1433,10 +1433,10 @@
         <v>100</v>
       </c>
       <c r="G13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="H13" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I13" t="s">
         <v>100</v>
@@ -1445,13 +1445,13 @@
         <v>75</v>
       </c>
       <c r="K13" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1459,10 +1459,10 @@
         <v>89</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D14">
         <v>43385</v>
@@ -1471,13 +1471,13 @@
         <v>99</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="G14" t="s">
         <v>109</v>
       </c>
       <c r="H14" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="I14" t="s">
         <v>100</v>
@@ -1486,10 +1486,10 @@
         <v>76</v>
       </c>
       <c r="K14" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="L14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="M14" t="s">
         <v>110</v>
@@ -11492,10 +11492,10 @@
     <mergeCell ref="G11:M11"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{8C1A18BA-69DA-A546-A7D4-0C3BC29F9A37}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{5EE18A43-A1AD-5D44-BE38-7503905C77CB}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J13:J14" xr:uid="{0A33A29C-588C-304B-887D-A424EC072D95}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J13:J14" xr:uid="{BD9B7B95-5B1E-CE43-B853-92795B5830EB}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11520,7 +11520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3:J4"/>
     </sheetView>
   </sheetViews>
@@ -21636,11 +21636,11 @@
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J3:J4" xr:uid="{507E2600-3B71-BE4A-B906-B111F31C4F01}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I3:I4" xr:uid="{5570860E-14C0-B645-95FA-3576DF6A28B9}">
+      <formula1>"Surface Stain,Intracellular"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J3:J4" xr:uid="{9E7F67F4-9618-7A4B-96E5-22D9FFACA35D}">
       <formula1>"Ignored,Used,Analysis Only"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I3:I4" xr:uid="{07A66728-FE01-B74A-B6EF-CC8CBFDDF6B4}">
-      <formula1>"Surface Stain,Intracellular"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Move 'injector' to preamble
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93EDA7B-AA0F-1C43-B741-5467856296EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B02028-D07B-E543-A87B-49B8240AEE6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="1760" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Name of Injector component used as part of the CyTOF software</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -135,40 +148,22 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Path to a file on a User's computer. 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>In .fcs format</t>
+          <t>Path to a file on a User's computer. 
+This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
+In .fcs format</t>
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -181,20 +176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Name of Injector component used as part of the CyTOF software</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -207,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -221,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -247,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -260,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -273,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="K12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -286,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="L12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -491,6 +473,12 @@
     <t>CyTOF batch identification number.</t>
   </si>
   <si>
+    <t>Injector</t>
+  </si>
+  <si>
+    <t>Name of Injector component used as part of the CyTOF software</t>
+  </si>
+  <si>
     <t>Section 'Run info' of tab 'Acquisition and Preprocessing'</t>
   </si>
   <si>
@@ -517,12 +505,6 @@
   </si>
   <si>
     <t>Date of CyTOF batch acquisition.</t>
-  </si>
-  <si>
-    <t>Injector</t>
-  </si>
-  <si>
-    <t>Name of Injector component used as part of the CyTOF software</t>
   </si>
   <si>
     <t>Acquisition_buffer</t>
@@ -717,13 +699,19 @@
     <t>XYZ1</t>
   </si>
   <si>
+    <t>HAT123</t>
+  </si>
+  <si>
     <t>CTTTPP111.00</t>
   </si>
   <si>
     <t>sample1_n.fcs</t>
   </si>
   <si>
-    <t>HAT123</t>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>sample2_n.fcs</t>
   </si>
   <si>
     <t>ABC</t>
@@ -742,12 +730,6 @@
   </si>
   <si>
     <t>a note like any other note</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2_n.fcs</t>
   </si>
   <si>
     <t>ABCD</t>
@@ -793,7 +775,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -820,6 +802,13 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -892,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -909,6 +898,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1247,16 +1237,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M2011"/>
+  <dimension ref="A1:L2012"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -1265,7 +1257,7 @@
       </c>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1276,7 +1268,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1287,7 +1279,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1298,7 +1290,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -1309,7 +1301,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1318,7 +1310,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1329,7 +1321,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -1340,161 +1332,157 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>83</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B11" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>86</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="K12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M11" s="3" t="s">
+      <c r="L12" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D12">
+      <c r="C13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="6">
         <v>43355</v>
       </c>
-      <c r="E12" t="s">
-        <v>96</v>
-      </c>
-      <c r="F12" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="E13" t="s">
         <v>99</v>
       </c>
-      <c r="I12" t="s">
-        <v>97</v>
-      </c>
-      <c r="J12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="F13" t="s">
         <v>100</v>
       </c>
-      <c r="L12" t="s">
+      <c r="G13" t="s">
         <v>101</v>
-      </c>
-      <c r="M12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" t="s">
-        <v>103</v>
-      </c>
-      <c r="C13" t="s">
-        <v>104</v>
-      </c>
-      <c r="D13">
-        <v>43385</v>
-      </c>
-      <c r="E13" t="s">
-        <v>96</v>
-      </c>
-      <c r="F13" t="s">
-        <v>105</v>
-      </c>
-      <c r="G13" t="s">
-        <v>106</v>
       </c>
       <c r="H13" t="s">
         <v>99</v>
       </c>
       <c r="I13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" t="s">
+        <v>102</v>
+      </c>
+      <c r="K13" t="s">
+        <v>103</v>
+      </c>
+      <c r="L13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J13" t="s">
+      <c r="C14" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="6">
+        <v>43385</v>
+      </c>
+      <c r="E14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H14" t="s">
+        <v>99</v>
+      </c>
+      <c r="I14" t="s">
         <v>74</v>
       </c>
-      <c r="K13" t="s">
-        <v>100</v>
-      </c>
-      <c r="L13" t="s">
-        <v>101</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="J14" t="s">
+        <v>102</v>
+      </c>
+      <c r="K14" t="s">
+        <v>103</v>
+      </c>
+      <c r="L14" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -11471,20 +11459,25 @@
     </row>
     <row r="2011" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2011" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2012" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="G10:M10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F11:L11"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{BDC80B24-1E72-4C4C-8B62-F0DAD564ACAC}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B01DAC3E-33C4-1845-9A07-BE5002F72D76}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J12:J13" xr:uid="{ABBBAF73-1F1A-FB43-9E56-E21E93A2DFCD}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I13:I14" xr:uid="{7785C63F-CBA0-1C44-B75C-34617221C9A2}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11497,7 +11490,7 @@
           <x14:formula1>
             <xm:f>'Data Dictionary'!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>J14:J2011</xm:sqref>
+          <xm:sqref>I15:I2012</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11509,7 +11502,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2002"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -21623,10 +21618,10 @@
     <mergeCell ref="B1:J1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J3:J4" xr:uid="{6F16D058-BEF7-4B4A-B330-B703E2AC687F}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J3:J4" xr:uid="{A8E21C94-D3F5-4742-839D-9FCAD732009A}">
       <formula1>"Ignored,Used,Analysis Only"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I3:I4" xr:uid="{D14CCBCC-1545-BB42-9A02-D995CEBF5853}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I3:I4" xr:uid="{6D3AD602-6FCF-6945-BC2E-EA187FC5F77B}">
       <formula1>"Surface Stain,Intracellular"</formula1>
     </dataValidation>
   </dataValidations>
@@ -21754,33 +21749,33 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="3" t="s">
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+    </row>
+    <row r="11" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move 'date_of_acquision' to preamble
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B02028-D07B-E543-A87B-49B8240AEE6F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FBD87A-0418-834F-9843-18C5A8BD3243}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color rgb="FF000000"/>
+            <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -135,7 +135,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Date of CyTOF batch acquisition.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -148,7 +161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -163,25 +176,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="D12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Date of CyTOF batch acquisition.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -189,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -229,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -255,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="K13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -413,7 +413,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4199" uniqueCount="118">
   <si>
     <t>LEGEND</t>
   </si>
@@ -479,6 +479,12 @@
     <t>Name of Injector component used as part of the CyTOF software</t>
   </si>
   <si>
+    <t>Date of acquisition</t>
+  </si>
+  <si>
+    <t>Date of CyTOF batch acquisition.</t>
+  </si>
+  <si>
     <t>Section 'Run info' of tab 'Acquisition and Preprocessing'</t>
   </si>
   <si>
@@ -499,12 +505,6 @@
   <si>
     <t>Path to a file on a User's computer. 
 This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.</t>
-  </si>
-  <si>
-    <t>Date of acquisition</t>
-  </si>
-  <si>
-    <t>Date of CyTOF batch acquisition.</t>
   </si>
   <si>
     <t>Acquisition_buffer</t>
@@ -702,18 +702,6 @@
     <t>HAT123</t>
   </si>
   <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>sample1_n.fcs</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2_n.fcs</t>
-  </si>
-  <si>
     <t>ABC</t>
   </si>
   <si>
@@ -739,6 +727,18 @@
   </si>
   <si>
     <t>a different note</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>sample2_n.fcs</t>
+  </si>
+  <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>sample1_n.fcs</t>
   </si>
   <si>
     <t>CD8</t>
@@ -798,17 +798,17 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -881,7 +881,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -895,10 +895,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1237,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2012"/>
+  <dimension ref="A1:K2013"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1248,16 +1251,16 @@
     <col min="1" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="5"/>
-    </row>
-    <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1268,7 +1271,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>82</v>
       </c>
@@ -1290,7 +1293,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -1301,7 +1304,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>82</v>
       </c>
@@ -1310,7 +1313,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:12" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -1321,7 +1324,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -1332,7 +1335,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -1343,146 +1346,142 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2">
+        <v>43355</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>83</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>86</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="K13" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="6" t="s">
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C14" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="E14" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="6">
-        <v>43355</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
+        <v>95</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" t="s">
         <v>99</v>
       </c>
-      <c r="F13" t="s">
+      <c r="K14" t="s">
         <v>100</v>
       </c>
-      <c r="G13" t="s">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" t="s">
+        <v>104</v>
+      </c>
+      <c r="C15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" t="s">
         <v>101</v>
       </c>
-      <c r="H13" t="s">
+      <c r="E15" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" t="s">
+        <v>95</v>
+      </c>
+      <c r="H15" t="s">
+        <v>74</v>
+      </c>
+      <c r="I15" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" t="s">
         <v>99</v>
       </c>
-      <c r="I13" t="s">
-        <v>73</v>
-      </c>
-      <c r="J13" t="s">
-        <v>102</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="K15" t="s">
         <v>103</v>
       </c>
-      <c r="L13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="6">
-        <v>43385</v>
-      </c>
-      <c r="E14" t="s">
-        <v>105</v>
-      </c>
-      <c r="F14" t="s">
-        <v>106</v>
-      </c>
-      <c r="G14" t="s">
-        <v>101</v>
-      </c>
-      <c r="H14" t="s">
-        <v>99</v>
-      </c>
-      <c r="I14" t="s">
-        <v>74</v>
-      </c>
-      <c r="J14" t="s">
-        <v>102</v>
-      </c>
-      <c r="K14" t="s">
-        <v>103</v>
-      </c>
-      <c r="L14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>87</v>
       </c>
@@ -11464,20 +11463,25 @@
     </row>
     <row r="2012" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2012" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2013" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2013" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:K12"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{B01DAC3E-33C4-1845-9A07-BE5002F72D76}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{16A4E294-B33D-7945-8FAE-A9ECED93F74B}">
       <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I13:I14" xr:uid="{7785C63F-CBA0-1C44-B75C-34617221C9A2}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H14:H15" xr:uid="{C805CC55-7035-F045-9E83-A0D21709AA9E}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11490,7 +11494,7 @@
           <x14:formula1>
             <xm:f>'Data Dictionary'!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I15:I2012</xm:sqref>
+          <xm:sqref>H16:H2013</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11503,7 +11507,7 @@
   <dimension ref="A1:J2002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11515,17 +11519,17 @@
       <c r="A1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -11563,31 +11567,31 @@
       <c r="A3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="6">
         <v>3983272</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="6" t="s">
         <v>78</v>
       </c>
     </row>
@@ -11595,31 +11599,31 @@
       <c r="A4" t="s">
         <v>87</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="6">
         <v>1231272</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="6" t="s">
         <v>79</v>
       </c>
     </row>
@@ -21617,14 +21621,6 @@
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J3:J4" xr:uid="{A8E21C94-D3F5-4742-839D-9FCAD732009A}">
-      <formula1>"Ignored,Used,Analysis Only"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I3:I4" xr:uid="{6D3AD602-6FCF-6945-BC2E-EA187FC5F77B}">
-      <formula1>"Surface Stain,Intracellular"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
@@ -21760,33 +21756,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="3" t="s">
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="12" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Move 'acquisition_buffer' to preamble
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FBD87A-0418-834F-9843-18C5A8BD3243}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730D4290-DA52-C448-919E-377B3B33231C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10200" yWindow="1260" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -148,7 +148,20 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Cell staining buffer used for antibody and cell dilution.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -161,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="C14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -176,20 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Cell staining buffer used for antibody and cell dilution.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="D14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="E14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -229,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="H14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -255,7 +255,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="I14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -413,7 +413,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4199" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4199" uniqueCount="117">
   <si>
     <t>LEGEND</t>
   </si>
@@ -485,6 +485,12 @@
     <t>Date of CyTOF batch acquisition.</t>
   </si>
   <si>
+    <t>Acquisition_buffer</t>
+  </si>
+  <si>
+    <t>Cell staining buffer used for antibody and cell dilution.</t>
+  </si>
+  <si>
     <t>Section 'Run info' of tab 'Acquisition and Preprocessing'</t>
   </si>
   <si>
@@ -505,12 +511,6 @@
   <si>
     <t>Path to a file on a User's computer. 
 This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.</t>
-  </si>
-  <si>
-    <t>Acquisition_buffer</t>
-  </si>
-  <si>
-    <t>Cell staining buffer used for antibody and cell dilution.</t>
   </si>
   <si>
     <t>Section 'Preprocessing' of tab 'Acquisition and Preprocessing'</t>
@@ -705,6 +705,18 @@
     <t>ABC</t>
   </si>
   <si>
+    <t>CTTTPP111.00</t>
+  </si>
+  <si>
+    <t>sample1_n.fcs</t>
+  </si>
+  <si>
+    <t>CTTTPP121.00</t>
+  </si>
+  <si>
+    <t>sample2_n.fcs</t>
+  </si>
+  <si>
     <t>sample1.fcs</t>
   </si>
   <si>
@@ -720,25 +732,10 @@
     <t>a note like any other note</t>
   </si>
   <si>
-    <t>ABCD</t>
-  </si>
-  <si>
     <t>sample2.fcs</t>
   </si>
   <si>
     <t>a different note</t>
-  </si>
-  <si>
-    <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2_n.fcs</t>
-  </si>
-  <si>
-    <t>CTTTPP111.00</t>
-  </si>
-  <si>
-    <t>sample1_n.fcs</t>
   </si>
   <si>
     <t>CD8</t>
@@ -798,6 +795,7 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -805,13 +803,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -842,8 +841,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2D2F6"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -877,11 +882,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -895,13 +909,19 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1240,10 +1260,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2013"/>
+  <dimension ref="A1:J2014"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1251,239 +1271,235 @@
     <col min="1" max="101" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="7" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>82</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>82</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="7" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>82</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="7">
         <v>43355</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="11" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>86</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B14" s="5" t="s">
+    <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D15" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" t="s">
+        <v>102</v>
+      </c>
+      <c r="I15" t="s">
+        <v>103</v>
+      </c>
+      <c r="J15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D16" t="s">
+        <v>105</v>
+      </c>
+      <c r="E16" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" t="s">
+        <v>103</v>
+      </c>
+      <c r="J16" t="s">
         <v>106</v>
-      </c>
-      <c r="C14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" t="s">
-        <v>97</v>
-      </c>
-      <c r="G14" t="s">
-        <v>95</v>
-      </c>
-      <c r="H14" t="s">
-        <v>73</v>
-      </c>
-      <c r="I14" t="s">
-        <v>98</v>
-      </c>
-      <c r="J14" t="s">
-        <v>99</v>
-      </c>
-      <c r="K14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E15" t="s">
-        <v>102</v>
-      </c>
-      <c r="F15" t="s">
-        <v>97</v>
-      </c>
-      <c r="G15" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" t="s">
-        <v>74</v>
-      </c>
-      <c r="I15" t="s">
-        <v>98</v>
-      </c>
-      <c r="J15" t="s">
-        <v>99</v>
-      </c>
-      <c r="K15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -11468,20 +11484,22 @@
     </row>
     <row r="2013" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2013" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2014" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2014" t="s">
         <v>87</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:K12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:J13"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C4" xr:uid="{16A4E294-B33D-7945-8FAE-A9ECED93F74B}">
-      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H14:H15" xr:uid="{C805CC55-7035-F045-9E83-A0D21709AA9E}">
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G15:G16" xr:uid="{DF95C6B9-4BD1-CA42-94FC-A18BB9A24250}">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11494,7 +11512,7 @@
           <x14:formula1>
             <xm:f>'Data Dictionary'!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H16:H2013</xm:sqref>
+          <xm:sqref>G17:G2014</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -11507,7 +11525,7 @@
   <dimension ref="A1:J2002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11519,17 +11537,17 @@
       <c r="A1" t="s">
         <v>83</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -11567,31 +11585,31 @@
       <c r="A3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="F3" s="9">
+        <v>3983272</v>
+      </c>
+      <c r="G3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="6">
-        <v>3983272</v>
-      </c>
-      <c r="G3" s="6" t="s">
+      <c r="H3" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="9" t="s">
         <v>78</v>
       </c>
     </row>
@@ -11599,31 +11617,31 @@
       <c r="A4" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="9">
+        <v>1231272</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F4" s="6">
-        <v>1231272</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="H4" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="I4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="9" t="s">
         <v>79</v>
       </c>
     </row>
@@ -21767,33 +21785,33 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="2:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
+    </row>
+    <row r="13" spans="2:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update example hardware version info
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1270219-0F18-DF4A-8634-55973DC39798}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6ACE777-E346-404E-AB36-E1B14336B56A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -793,9 +793,6 @@
     <t>ABC</t>
   </si>
   <si>
-    <t>3.0.2</t>
-  </si>
-  <si>
     <t>CTTTPP111.00</t>
   </si>
   <si>
@@ -857,6 +854,9 @@
   </si>
   <si>
     <t>146Nb</t>
+  </si>
+  <si>
+    <t>Fluidigm 3.0.2</t>
   </si>
 </sst>
 </file>
@@ -1000,9 +1000,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1013,6 +1010,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1354,7 +1354,7 @@
   <dimension ref="A1:J2018"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1366,10 +1366,10 @@
       <c r="A1" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1378,7 +1378,7 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1389,7 +1389,7 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1411,7 +1411,7 @@
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1422,7 +1422,7 @@
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7"/>
+      <c r="C6" s="6"/>
     </row>
     <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1431,7 +1431,7 @@
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1442,7 +1442,7 @@
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1453,7 +1453,7 @@
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1464,7 +1464,7 @@
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>43355</v>
       </c>
     </row>
@@ -1475,7 +1475,7 @@
       <c r="B11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1520,26 +1520,26 @@
         <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
@@ -1577,17 +1577,17 @@
       <c r="A19" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" t="s">
         <v>109</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>110</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>111</v>
-      </c>
-      <c r="E19" t="s">
-        <v>112</v>
       </c>
       <c r="F19" t="s">
         <v>107</v>
@@ -1596,13 +1596,13 @@
         <v>85</v>
       </c>
       <c r="H19" t="s">
+        <v>112</v>
+      </c>
+      <c r="I19" t="s">
         <v>113</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>114</v>
-      </c>
-      <c r="J19" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1610,16 +1610,16 @@
         <v>99</v>
       </c>
       <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
         <v>116</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>117</v>
       </c>
-      <c r="D20" t="s">
-        <v>118</v>
-      </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
         <v>107</v>
@@ -1628,13 +1628,13 @@
         <v>86</v>
       </c>
       <c r="H20" t="s">
+        <v>112</v>
+      </c>
+      <c r="I20" t="s">
         <v>113</v>
       </c>
-      <c r="I20" t="s">
-        <v>114</v>
-      </c>
       <c r="J20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -11675,17 +11675,17 @@
       <c r="A1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -11723,31 +11723,31 @@
       <c r="A3" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="8">
+        <v>3983272</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="F3" s="9">
-        <v>3983272</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>90</v>
       </c>
     </row>
@@ -11755,31 +11755,31 @@
       <c r="A4" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>122</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="8">
+        <v>1231272</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="F4" s="9">
-        <v>1231272</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
merge debarcoding method & protocol
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6F2D06-4DE6-1C45-8926-CC2E778447EF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D082BDBB-69DA-684F-9557-D7871C140A20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -193,7 +193,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -206,7 +206,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -245,13 +245,31 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a User's computer. 
-This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
-In .fcs format</t>
+          <t xml:space="preserve">Path to a file on a User's computer. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
         </r>
       </text>
     </comment>
@@ -260,12 +278,21 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Path to a file on a user's computer.
-In .fcs format</t>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
         </r>
       </text>
     </comment>
@@ -308,20 +335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>The strategy/kit used to barcode CyTOF samples.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -334,12 +348,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="I19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -479,7 +493,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4235" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4232" uniqueCount="130">
   <si>
     <t>LEGEND</t>
   </si>
@@ -825,9 +839,6 @@
     <t>GHIL</t>
   </si>
   <si>
-    <t>FLUIDIGM XYZ</t>
-  </si>
-  <si>
     <t>FLUIDIGM 1234</t>
   </si>
   <si>
@@ -880,7 +891,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -916,6 +927,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1017,9 +1034,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1030,6 +1044,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1368,25 +1385,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2019"/>
+  <dimension ref="A1:I2019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:J21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="101" width="30.6640625" customWidth="1"/>
+    <col min="1" max="100" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C1" s="5"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1395,7 +1412,7 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1406,7 +1423,7 @@
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1417,7 +1434,7 @@
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1428,7 +1445,7 @@
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1439,7 +1456,7 @@
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1459,7 +1476,7 @@
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>106</v>
       </c>
     </row>
@@ -1479,7 +1496,7 @@
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1490,7 +1507,7 @@
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6">
         <v>43355</v>
       </c>
     </row>
@@ -1501,7 +1518,7 @@
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1532,7 +1549,7 @@
         <v>95</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>84</v>
@@ -1549,25 +1566,24 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="9"/>
+      <c r="D18" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>99</v>
       </c>
@@ -1590,20 +1606,17 @@
         <v>49</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="J19" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>100</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>110</v>
       </c>
       <c r="C20" t="s">
@@ -1627,22 +1640,19 @@
       <c r="I20" t="s">
         <v>115</v>
       </c>
-      <c r="J20" t="s">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>117</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>118</v>
-      </c>
-      <c r="D21" t="s">
-        <v>119</v>
       </c>
       <c r="E21" t="s">
         <v>113</v>
@@ -1657,63 +1667,60 @@
         <v>114</v>
       </c>
       <c r="I21" t="s">
-        <v>115</v>
-      </c>
-      <c r="J21" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>100</v>
       </c>
@@ -11657,7 +11664,7 @@
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="D18:I18"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{A739248F-A17F-8249-83A3-57F11FD24917}">
@@ -11701,17 +11708,17 @@
       <c r="A1" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -11749,31 +11756,31 @@
       <c r="A3" t="s">
         <v>100</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="8">
+        <v>3983272</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="F3" s="9">
-        <v>3983272</v>
-      </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="H3" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="8" t="s">
         <v>91</v>
       </c>
     </row>
@@ -11781,31 +11788,31 @@
       <c r="A4" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="F4" s="8">
+        <v>1231272</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="F4" s="9">
-        <v>1231272</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
regenrate template with new tabs
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5433B45C-CBFD-6943-B1C1-F57B346C5D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDE621B-FBE9-E443-AD5C-5CEEE6F0B74B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="2160" windowWidth="19120" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
     <sheet name="Antibody Information" sheetId="2" r:id="rId2"/>
-    <sheet name="Legend" sheetId="3" r:id="rId3"/>
-    <sheet name="Data Dictionary" sheetId="4" r:id="rId4"/>
+    <sheet name="Controls and Spike-Ins" sheetId="5" r:id="rId3"/>
+    <sheet name="Barcoding" sheetId="6" r:id="rId4"/>
+    <sheet name="Legend" sheetId="3" r:id="rId5"/>
+    <sheet name="Data Dictionary" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -85,7 +87,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -93,55 +95,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a User's computer. 
-This file contains the normalized &amp; debarcoded spike-in for a batch.
-In .fcs format</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a user's computer.
-In .fcs format</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a user's computer.
-In .fcs format</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -149,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+    <comment ref="B8" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -162,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -175,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -188,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -201,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -214,7 +173,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
+    <comment ref="B13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -227,20 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -259,7 +205,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">This .fcs file is an intermediate file that has been normalized, concatenated, and debarcoded, but has the veri-cells and has not been cleaned up.
+          <t xml:space="preserve">This file contains the normalized &amp; debarcoded spike-in for a batch.
 </t>
         </r>
         <r>
@@ -273,7 +219,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
+    <comment ref="B15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -296,7 +242,43 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
+    <comment ref="B18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formatted as C????????.??</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C18" authorId="0" shapeId="0" xr:uid="{DC2EA13B-4569-3D4D-B359-E5663D18CDB6}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Path to a file on a user's computer.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>In .fcs format</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0" shapeId="0" xr:uid="{4F14E1CB-3AD3-A94B-91E2-D472B4D9670F}">
       <text>
         <r>
           <rPr>
@@ -309,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
+    <comment ref="E18" authorId="0" shapeId="0" xr:uid="{A6B354D6-AC8C-B144-8C74-ADB29FD8B585}">
       <text>
         <r>
           <rPr>
@@ -322,20 +304,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{5FD5B33B-FDA8-2D46-AD13-77BF21A9A974}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>An ID that maps to the specific isotope labeling scheme in the debarcoding protocol.</t>
+          <t>Any notes pertaining to preprocessing of CyTOF data.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
+    <comment ref="G18" authorId="0" shapeId="0" xr:uid="{9E003301-7024-2740-9938-D3DA7A25C8A3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Any notes pertaining to preprocessing of CyTOF data.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -479,8 +474,145 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>CIDC</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{0426593C-2D6C-7B4C-89FB-1DC9316371DA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody type collected for this study.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{FCE0E859-91AF-1C4A-8968-C8EE4B60DC75}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Resulting type of antibody clone from primary antibody sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{4A30D50A-808D-C143-8C6A-2719D62F2592}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Company from which antibody sample was derived.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{9B3E29B9-80D9-384F-97BB-5BC80D4497E3}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody registry catalog number assigned to antibody sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{9747EE88-54FF-164D-A7A2-57F4D03C5007}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Identification number assigned to the particular quantity or lot of material from manufacturer.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{294E7154-381F-9D4B-AF49-FECD8CE732CA}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody isotype used to help differentiate antibody signals.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>CIDC</author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{C98B5137-E7E9-6A49-A3C7-F0CC1A7311A5}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Antibody type collected for this study.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{A71EA9BF-319C-2C47-A6E0-507AFF0D4982}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Resulting type of antibody clone from primary antibody sample.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{21D4016C-D5C8-CF42-950A-1B3F27D08364}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Company from which antibody sample was derived.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4229" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4594" uniqueCount="136">
   <si>
     <t>LEGEND</t>
   </si>
@@ -814,25 +946,16 @@
     <t>CTTTPP111.00</t>
   </si>
   <si>
-    <t>sample1_n.fcs</t>
-  </si>
-  <si>
     <t>sample1.fcs</t>
   </si>
   <si>
     <t>GHIL</t>
   </si>
   <si>
-    <t>FLUIDIGM 1234</t>
-  </si>
-  <si>
     <t>a note like any other note</t>
   </si>
   <si>
     <t>CTTTPP121.00</t>
-  </si>
-  <si>
-    <t>sample2_n.fcs</t>
   </si>
   <si>
     <t>sample2.fcs</t>
@@ -872,6 +995,33 @@
   </si>
   <si>
     <t>Metadata file for cytof_10021_9204</t>
+  </si>
+  <si>
+    <t>Concatenated Spike in fcs filename</t>
+  </si>
+  <si>
+    <t>Concatenated Raw fcs filename(s)</t>
+  </si>
+  <si>
+    <t>Controls info</t>
+  </si>
+  <si>
+    <t>Control name</t>
+  </si>
+  <si>
+    <t>Cimac participant id</t>
+  </si>
+  <si>
+    <t>Spike-in fcs filename</t>
+  </si>
+  <si>
+    <t>Id (cimac id/participant id/control name</t>
+  </si>
+  <si>
+    <t>Barcoding</t>
+  </si>
+  <si>
+    <t>Barcode number</t>
   </si>
 </sst>
 </file>
@@ -960,7 +1110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1003,11 +1153,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1032,7 +1206,26 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1372,10 +1565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2019"/>
+  <dimension ref="A1:H2018"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1383,16 +1576,16 @@
     <col min="1" max="99" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="14"/>
+    </row>
+    <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>94</v>
       </c>
@@ -1403,7 +1596,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>94</v>
       </c>
@@ -1414,7 +1607,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1425,7 +1618,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1436,7 +1629,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>94</v>
       </c>
@@ -1447,205 +1640,195 @@
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>94</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6">
+        <v>43355</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>94</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>94</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C10" s="2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="6">
-        <v>43355</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>94</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+    </row>
+    <row r="13" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>94</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>94</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>94</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>108</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>98</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>109</v>
+      <c r="B20" t="s">
+        <v>113</v>
       </c>
       <c r="C20" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D20" t="s">
         <v>111</v>
       </c>
       <c r="E20" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="F20" t="s">
-        <v>107</v>
-      </c>
-      <c r="G20" t="s">
-        <v>113</v>
-      </c>
-      <c r="H20" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>99</v>
       </c>
-      <c r="B21" t="s">
-        <v>115</v>
-      </c>
-      <c r="C21" t="s">
-        <v>116</v>
-      </c>
-      <c r="D21" t="s">
-        <v>117</v>
-      </c>
-      <c r="E21" t="s">
-        <v>112</v>
-      </c>
-      <c r="F21" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21" t="s">
-        <v>113</v>
-      </c>
-      <c r="H21" t="s">
-        <v>118</v>
-      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
@@ -11632,19 +11815,13 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2019" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2019" t="s">
-        <v>99</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13" xr:uid="{A739248F-A17F-8249-83A3-57F11FD24917}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{A739248F-A17F-8249-83A3-57F11FD24917}">
       <formula1>"True,False"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11657,8 +11834,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11670,17 +11847,17 @@
       <c r="A1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -11719,25 +11896,25 @@
         <v>99</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>122</v>
       </c>
       <c r="F3" s="8">
         <v>3983272</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I3" s="8" t="s">
         <v>88</v>
@@ -11751,25 +11928,25 @@
         <v>99</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F4" s="8">
         <v>1231272</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>88</v>
@@ -21796,6 +21973,1914 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD29E0F0-5D53-2F4B-A1C9-4CD3DD60A420}">
+  <dimension ref="A1:G323"/>
+  <sheetViews>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection sqref="A1:XFD39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A134" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A135" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A151" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A152" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A154" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A158" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A160" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A161" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A162" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A163" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A164" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A165" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A166" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A168" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A169" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A170" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A171" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A172" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A173" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A174" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A175" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A176" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A177" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A242" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A243" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A244" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A245" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A246" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A247" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A248" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A249" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A250" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A251" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A252" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A253" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A254" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A255" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A256" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A257" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A258" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A259" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A260" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A261" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A262" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A263" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A264" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A265" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A266" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A267" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A268" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A269" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A270" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A271" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A272" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A273" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A274" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A275" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A276" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A277" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A278" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A279" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A280" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A281" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A282" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A283" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A284" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A285" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A287" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A288" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A289" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A290" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A291" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A292" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A293" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A294" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A295" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A296" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A297" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A298" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A299" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A300" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A301" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A303" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A304" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A305" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A306" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A307" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A308" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A309" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A310" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A311" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A312" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A313" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A314" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A323" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F51589B-9409-2547-AE0A-0DC8FCD08214}">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="33.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:E39"/>
   <sheetViews>
@@ -22226,7 +24311,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:G5"/>
   <sheetViews>

</xml_diff>

<commit_message>
add example test data for barcodes and controls
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D620635C-7BC2-A74E-9876-9BED72373E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98908FDA-2990-8946-BF3C-C473F32903B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="2160" windowWidth="19120" windowHeight="8940" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -485,7 +485,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -612,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4594" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4599" uniqueCount="140">
   <si>
     <t>LEGEND</t>
   </si>
@@ -1023,6 +1023,18 @@
   <si>
     <t>Id (cimac id/participant id/control name)</t>
   </si>
+  <si>
+    <t>CTTTPP111</t>
+  </si>
+  <si>
+    <t>ABC123</t>
+  </si>
+  <si>
+    <t>XYZ1-control</t>
+  </si>
+  <si>
+    <t>XYZ1-control.fcs</t>
+  </si>
 </sst>
 </file>
 
@@ -1181,7 +1193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1226,6 +1238,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2018"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21976,8 +21991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD29E0F0-5D53-2F4B-A1C9-4CD3DD60A420}">
   <dimension ref="A1:G323"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection sqref="A1:XFD39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22030,9 +22045,13 @@
       <c r="A3" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="17" t="s">
+        <v>138</v>
+      </c>
       <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="D3" s="17" t="s">
+        <v>139</v>
+      </c>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -23648,8 +23667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F51589B-9409-2547-AE0A-0DC8FCD08214}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23683,13 +23702,19 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B3" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">

</xml_diff>

<commit_message>
add preamble row to controls tab
</commit_message>
<xml_diff>
--- a/template_examples/cytof_template.xlsx
+++ b/template_examples/cytof_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rbiswas/VSCodeProjects/cidc-schemas/template_examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98908FDA-2990-8946-BF3C-C473F32903B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00551E61-21D4-8E44-8599-9377F0D5824E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -48,7 +48,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -61,7 +61,7 @@
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -480,7 +480,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{0426593C-2D6C-7B4C-89FB-1DC9316371DA}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{0426593C-2D6C-7B4C-89FB-1DC9316371DA}">
       <text>
         <r>
           <rPr>
@@ -493,7 +493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{FCE0E859-91AF-1C4A-8968-C8EE4B60DC75}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{FCE0E859-91AF-1C4A-8968-C8EE4B60DC75}">
       <text>
         <r>
           <rPr>
@@ -506,12 +506,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{4A30D50A-808D-C143-8C6A-2719D62F2592}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{4A30D50A-808D-C143-8C6A-2719D62F2592}">
       <text>
         <r>
           <rPr>
             <sz val="10"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -519,7 +519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{9B3E29B9-80D9-384F-97BB-5BC80D4497E3}">
+    <comment ref="E4" authorId="0" shapeId="0" xr:uid="{9B3E29B9-80D9-384F-97BB-5BC80D4497E3}">
       <text>
         <r>
           <rPr>
@@ -532,7 +532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{9747EE88-54FF-164D-A7A2-57F4D03C5007}">
+    <comment ref="F4" authorId="0" shapeId="0" xr:uid="{9747EE88-54FF-164D-A7A2-57F4D03C5007}">
       <text>
         <r>
           <rPr>
@@ -545,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{294E7154-381F-9D4B-AF49-FECD8CE732CA}">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{294E7154-381F-9D4B-AF49-FECD8CE732CA}">
       <text>
         <r>
           <rPr>
@@ -568,7 +568,7 @@
     <author>CIDC</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0" shapeId="0" xr:uid="{C98B5137-E7E9-6A49-A3C7-F0CC1A7311A5}">
+    <comment ref="B4" authorId="0" shapeId="0" xr:uid="{C98B5137-E7E9-6A49-A3C7-F0CC1A7311A5}">
       <text>
         <r>
           <rPr>
@@ -581,7 +581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C2" authorId="0" shapeId="0" xr:uid="{A71EA9BF-319C-2C47-A6E0-507AFF0D4982}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{A71EA9BF-319C-2C47-A6E0-507AFF0D4982}">
       <text>
         <r>
           <rPr>
@@ -594,7 +594,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{21D4016C-D5C8-CF42-950A-1B3F27D08364}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{21D4016C-D5C8-CF42-950A-1B3F27D08364}">
       <text>
         <r>
           <rPr>
@@ -612,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4599" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4605" uniqueCount="140">
   <si>
     <t>LEGEND</t>
   </si>
@@ -1122,7 +1122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1189,11 +1189,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1230,6 +1295,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1239,8 +1314,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1583,7 +1667,7 @@
   <dimension ref="A1:H2018"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1595,10 +1679,10 @@
       <c r="A1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="C1" s="14"/>
+      <c r="C1" s="18"/>
     </row>
     <row r="2" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1767,12 +1851,12 @@
       <c r="B17" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
@@ -11835,7 +11919,7 @@
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="C17:F17"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10" xr:uid="{A739248F-A17F-8249-83A3-57F11FD24917}">
       <formula1>"True,False"</formula1>
     </dataValidation>
@@ -11849,7 +11933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J2002"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -11862,17 +11946,17 @@
       <c r="A1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -21989,15 +22073,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD29E0F0-5D53-2F4B-A1C9-4CD3DD60A420}">
-  <dimension ref="A1:G323"/>
+  <dimension ref="A1:H325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
@@ -22005,119 +22090,136 @@
     <col min="7" max="7" width="19.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="17" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="17" t="s">
+      <c r="C5" s="8"/>
+      <c r="D5" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="8"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>99</v>
       </c>
+      <c r="E16" s="16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
@@ -23651,6 +23753,16 @@
     </row>
     <row r="323" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
         <v>99</v>
       </c>
     </row>
@@ -23665,118 +23777,134 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F51589B-9409-2547-AE0A-0DC8FCD08214}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5" customWidth="1"/>
     <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+    </row>
+    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="7" t="s">
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D5" s="8" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -23893,6 +24021,16 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>